<commit_message>
Capítulo 1 de Filipenses corregido
</commit_message>
<xml_diff>
--- a/documentation/books.xlsx
+++ b/documentation/books.xlsx
@@ -23,11 +23,11 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$71</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$71</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$71</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$71</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$72</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$71</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$71</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$72</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
@@ -46,17 +46,18 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -1102,7 +1103,7 @@
   </sheetPr>
   <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E51" activeCellId="0" sqref="E51"/>
     </sheetView>
   </sheetViews>
@@ -2583,7 +2584,7 @@
       <c r="D51" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="E51" s="0" t="s">
+      <c r="E51" s="2" t="s">
         <v>162</v>
       </c>
       <c r="F51" s="0" t="s">

</xml_diff>

<commit_message>
Filipenses integrado en archivo general
</commit_message>
<xml_diff>
--- a/documentation/books.xlsx
+++ b/documentation/books.xlsx
@@ -24,12 +24,12 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$71</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$71</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$71</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$71</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$71</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$72</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$71</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$72</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
@@ -47,17 +47,19 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$B$1:$I$67</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -368,6 +370,9 @@
     <t xml:space="preserve">Amós</t>
   </si>
   <si>
+    <t xml:space="preserve">*</t>
+  </si>
+  <si>
     <t xml:space="preserve">Amos</t>
   </si>
   <si>
@@ -555,9 +560,6 @@
   </si>
   <si>
     <t xml:space="preserve">Filipenses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*</t>
   </si>
   <si>
     <t xml:space="preserve">Philippians</t>
@@ -736,7 +738,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -835,6 +837,13 @@
     <font>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -987,9 +996,13 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -998,6 +1011,22 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1103,8 +1132,8 @@
   </sheetPr>
   <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E51" activeCellId="0" sqref="E51"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I72" activeCellId="0" sqref="I72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1113,7 +1142,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.69"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="5.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="5.15"/>
@@ -1125,28 +1154,28 @@
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1163,7 +1192,7 @@
       <c r="D2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F2" s="0" t="s">
@@ -1192,7 +1221,7 @@
       <c r="D3" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F3" s="0" t="s">
@@ -1221,7 +1250,7 @@
       <c r="D4" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>0</v>
       </c>
       <c r="F4" s="0" t="s">
@@ -1250,7 +1279,7 @@
       <c r="D5" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>0</v>
       </c>
       <c r="F5" s="0" t="s">
@@ -1279,7 +1308,7 @@
       <c r="D6" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>0</v>
       </c>
       <c r="F6" s="0" t="s">
@@ -1308,7 +1337,7 @@
       <c r="D7" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F7" s="0" t="s">
@@ -1337,7 +1366,7 @@
       <c r="D8" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="2" t="n">
+      <c r="E8" s="3" t="n">
         <v>1</v>
       </c>
       <c r="F8" s="0" t="s">
@@ -1366,7 +1395,7 @@
       <c r="D9" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F9" s="0" t="s">
@@ -1395,7 +1424,7 @@
       <c r="D10" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F10" s="0" t="s">
@@ -1424,7 +1453,7 @@
       <c r="D11" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F11" s="0" t="s">
@@ -1453,7 +1482,7 @@
       <c r="D12" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="1" t="n">
         <v>0</v>
       </c>
       <c r="F12" s="0" t="s">
@@ -1482,7 +1511,7 @@
       <c r="D13" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="1" t="n">
         <v>0</v>
       </c>
       <c r="F13" s="0" t="s">
@@ -1511,7 +1540,7 @@
       <c r="D14" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="1" t="n">
         <v>0</v>
       </c>
       <c r="F14" s="0" t="s">
@@ -1540,7 +1569,7 @@
       <c r="D15" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="1" t="n">
         <v>0</v>
       </c>
       <c r="F15" s="0" t="s">
@@ -1569,7 +1598,7 @@
       <c r="D16" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F16" s="0" t="s">
@@ -1598,7 +1627,7 @@
       <c r="D17" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="E17" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F17" s="0" t="s">
@@ -1627,7 +1656,7 @@
       <c r="D18" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="E18" s="1" t="n">
         <v>0</v>
       </c>
       <c r="F18" s="0" t="s">
@@ -1656,7 +1685,7 @@
       <c r="D19" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="0" t="n">
+      <c r="E19" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F19" s="0" t="s">
@@ -1685,7 +1714,7 @@
       <c r="D20" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="0" t="n">
+      <c r="E20" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F20" s="0" t="s">
@@ -1714,7 +1743,7 @@
       <c r="D21" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="0" t="n">
+      <c r="E21" s="1" t="n">
         <v>0</v>
       </c>
       <c r="F21" s="0" t="s">
@@ -1743,7 +1772,7 @@
       <c r="D22" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E22" s="0" t="n">
+      <c r="E22" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F22" s="0" t="s">
@@ -1772,7 +1801,7 @@
       <c r="D23" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E23" s="0" t="n">
+      <c r="E23" s="1" t="n">
         <v>0</v>
       </c>
       <c r="F23" s="0" t="s">
@@ -1801,7 +1830,7 @@
       <c r="D24" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E24" s="0" t="n">
+      <c r="E24" s="1" t="n">
         <v>0</v>
       </c>
       <c r="F24" s="0" t="s">
@@ -1830,7 +1859,7 @@
       <c r="D25" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="0" t="n">
+      <c r="E25" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F25" s="0" t="s">
@@ -1859,7 +1888,7 @@
       <c r="D26" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E26" s="0" t="n">
+      <c r="E26" s="1" t="n">
         <v>0</v>
       </c>
       <c r="F26" s="0" t="s">
@@ -1888,7 +1917,7 @@
       <c r="D27" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E27" s="0" t="n">
+      <c r="E27" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F27" s="0" t="s">
@@ -1917,7 +1946,7 @@
       <c r="D28" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E28" s="0" t="n">
+      <c r="E28" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F28" s="0" t="s">
@@ -1946,7 +1975,7 @@
       <c r="D29" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E29" s="0" t="n">
+      <c r="E29" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F29" s="0" t="s">
@@ -1975,7 +2004,7 @@
       <c r="D30" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E30" s="0" t="n">
+      <c r="E30" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F30" s="0" t="s">
@@ -2004,14 +2033,14 @@
       <c r="D31" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E31" s="0" t="n">
-        <v>0</v>
+      <c r="E31" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H31" s="0" t="n">
         <v>9</v>
@@ -2028,19 +2057,19 @@
         <v>31</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D32" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E32" s="0" t="n">
+      <c r="E32" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H32" s="0" t="n">
         <v>1</v>
@@ -2057,19 +2086,19 @@
         <v>32</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D33" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E33" s="0" t="n">
+      <c r="E33" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H33" s="0" t="n">
         <v>4</v>
@@ -2086,19 +2115,19 @@
         <v>33</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E34" s="0" t="n">
+      <c r="E34" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H34" s="0" t="n">
         <v>7</v>
@@ -2115,19 +2144,19 @@
         <v>34</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D35" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E35" s="0" t="n">
+      <c r="E35" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H35" s="0" t="n">
         <v>3</v>
@@ -2144,19 +2173,19 @@
         <v>35</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D36" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E36" s="0" t="n">
+      <c r="E36" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H36" s="0" t="n">
         <v>3</v>
@@ -2173,19 +2202,19 @@
         <v>36</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D37" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E37" s="0" t="n">
+      <c r="E37" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H37" s="0" t="n">
         <v>3</v>
@@ -2202,19 +2231,19 @@
         <v>37</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D38" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="0" t="n">
+      <c r="E38" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H38" s="0" t="n">
         <v>2</v>
@@ -2231,19 +2260,19 @@
         <v>38</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D39" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="0" t="n">
+      <c r="E39" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H39" s="0" t="n">
         <v>14</v>
@@ -2260,19 +2289,19 @@
         <v>39</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D40" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E40" s="0" t="n">
+      <c r="E40" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H40" s="0" t="n">
         <v>4</v>
@@ -2289,25 +2318,25 @@
         <v>40</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="E41" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="E41" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H41" s="0" t="n">
         <v>28</v>
       </c>
       <c r="I41" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2318,25 +2347,25 @@
         <v>41</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="E42" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="E42" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H42" s="0" t="n">
         <v>16</v>
       </c>
       <c r="I42" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2347,25 +2376,25 @@
         <v>42</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="E43" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="E43" s="1" t="n">
         <v>0</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H43" s="0" t="n">
         <v>24</v>
       </c>
       <c r="I43" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2376,25 +2405,25 @@
         <v>43</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="E44" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="E44" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H44" s="0" t="n">
         <v>21</v>
       </c>
       <c r="I44" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2405,25 +2434,25 @@
         <v>44</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="E45" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="E45" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H45" s="0" t="n">
         <v>28</v>
       </c>
       <c r="I45" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2434,25 +2463,25 @@
         <v>45</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="E46" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="E46" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H46" s="0" t="n">
         <v>16</v>
       </c>
       <c r="I46" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2463,25 +2492,25 @@
         <v>46</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="E47" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="E47" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H47" s="0" t="n">
         <v>16</v>
       </c>
       <c r="I47" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2492,25 +2521,25 @@
         <v>47</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="E48" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="E48" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H48" s="0" t="n">
         <v>13</v>
       </c>
       <c r="I48" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2521,25 +2550,25 @@
         <v>48</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="E49" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="E49" s="1" t="n">
         <v>0</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H49" s="0" t="n">
         <v>6</v>
       </c>
       <c r="I49" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2550,25 +2579,25 @@
         <v>49</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="E50" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="E50" s="1" t="n">
         <v>0</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="G50" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H50" s="0" t="n">
         <v>6</v>
       </c>
       <c r="I50" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2579,13 +2608,13 @@
         <v>50</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>162</v>
+        <v>130</v>
+      </c>
+      <c r="E51" s="3" t="n">
+        <v>1</v>
       </c>
       <c r="F51" s="0" t="s">
         <v>163</v>
@@ -2597,7 +2626,7 @@
         <v>4</v>
       </c>
       <c r="I51" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2611,9 +2640,9 @@
         <v>165</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="E52" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="E52" s="1" t="n">
         <v>0</v>
       </c>
       <c r="F52" s="0" t="s">
@@ -2626,7 +2655,7 @@
         <v>4</v>
       </c>
       <c r="I52" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2640,9 +2669,9 @@
         <v>168</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="E53" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="E53" s="1" t="n">
         <v>0</v>
       </c>
       <c r="F53" s="0" t="s">
@@ -2655,7 +2684,7 @@
         <v>5</v>
       </c>
       <c r="I53" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2669,9 +2698,9 @@
         <v>171</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="E54" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="E54" s="1" t="n">
         <v>0</v>
       </c>
       <c r="F54" s="0" t="s">
@@ -2684,7 +2713,7 @@
         <v>3</v>
       </c>
       <c r="I54" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2698,9 +2727,9 @@
         <v>174</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="E55" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="E55" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F55" s="0" t="s">
@@ -2713,7 +2742,7 @@
         <v>6</v>
       </c>
       <c r="I55" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2727,9 +2756,9 @@
         <v>177</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="E56" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="E56" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F56" s="0" t="s">
@@ -2742,7 +2771,7 @@
         <v>4</v>
       </c>
       <c r="I56" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2756,9 +2785,9 @@
         <v>180</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="E57" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="E57" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F57" s="0" t="s">
@@ -2771,7 +2800,7 @@
         <v>3</v>
       </c>
       <c r="I57" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2785,9 +2814,9 @@
         <v>183</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="E58" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="E58" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F58" s="0" t="s">
@@ -2800,7 +2829,7 @@
         <v>1</v>
       </c>
       <c r="I58" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2814,9 +2843,9 @@
         <v>186</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="E59" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="E59" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F59" s="0" t="s">
@@ -2829,7 +2858,7 @@
         <v>13</v>
       </c>
       <c r="I59" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2843,9 +2872,9 @@
         <v>189</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="E60" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="E60" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F60" s="0" t="s">
@@ -2858,7 +2887,7 @@
         <v>5</v>
       </c>
       <c r="I60" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2872,9 +2901,9 @@
         <v>192</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="E61" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="E61" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F61" s="0" t="s">
@@ -2887,7 +2916,7 @@
         <v>5</v>
       </c>
       <c r="I61" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2901,9 +2930,9 @@
         <v>195</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="E62" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="E62" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F62" s="0" t="s">
@@ -2916,7 +2945,7 @@
         <v>3</v>
       </c>
       <c r="I62" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2930,9 +2959,9 @@
         <v>198</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="E63" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="E63" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F63" s="0" t="s">
@@ -2945,7 +2974,7 @@
         <v>5</v>
       </c>
       <c r="I63" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2959,9 +2988,9 @@
         <v>201</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="E64" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="E64" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F64" s="0" t="s">
@@ -2974,7 +3003,7 @@
         <v>1</v>
       </c>
       <c r="I64" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2988,9 +3017,9 @@
         <v>204</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="E65" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="E65" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F65" s="0" t="s">
@@ -3003,7 +3032,7 @@
         <v>1</v>
       </c>
       <c r="I65" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3017,9 +3046,9 @@
         <v>207</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="E66" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="E66" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F66" s="0" t="s">
@@ -3032,7 +3061,7 @@
         <v>1</v>
       </c>
       <c r="I66" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3046,9 +3075,9 @@
         <v>210</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="E67" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="E67" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F67" s="0" t="s">
@@ -3065,10 +3094,10 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E68" s="0" t="n">
+      <c r="E68" s="4" t="n">
         <v>66</v>
       </c>
-      <c r="H68" s="0" t="n">
+      <c r="H68" s="4" t="n">
         <f aca="false">SUM(H2:H67)</f>
         <v>1189</v>
       </c>
@@ -3077,41 +3106,41 @@
       <c r="D69" s="0" t="s">
         <v>213</v>
       </c>
-      <c r="E69" s="0" t="n">
+      <c r="E69" s="4" t="n">
         <f aca="false">COUNTIF(E2:E67,1)</f>
-        <v>46</v>
-      </c>
-      <c r="H69" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="H69" s="5" t="n">
         <f aca="false">SUMIF(E2:E67,1,H2:H67)+75</f>
-        <v>874</v>
+        <v>878</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D70" s="0" t="s">
         <v>214</v>
       </c>
-      <c r="E70" s="3" t="n">
+      <c r="E70" s="6" t="n">
         <f aca="false">E69/E68</f>
-        <v>0.696969696969697</v>
-      </c>
-      <c r="F70" s="3"/>
-      <c r="G70" s="3"/>
-      <c r="H70" s="3" t="n">
+        <v>0.712121212121212</v>
+      </c>
+      <c r="F70" s="7"/>
+      <c r="G70" s="7"/>
+      <c r="H70" s="6" t="n">
         <f aca="false">H69/H68</f>
-        <v>0.735071488645921</v>
+        <v>0.738435660218671</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D71" s="0" t="s">
         <v>215</v>
       </c>
-      <c r="E71" s="0" t="n">
+      <c r="E71" s="4" t="n">
         <f aca="false">COUNTIF(E2:E69,0)</f>
-        <v>19</v>
-      </c>
-      <c r="H71" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="H71" s="5" t="n">
         <f aca="false">SUMIF(E2:E67,0,H2:H67)+75</f>
-        <v>461</v>
+        <v>452</v>
       </c>
     </row>
   </sheetData>
@@ -3147,7 +3176,7 @@
       <c r="A2" s="0" t="s">
         <v>216</v>
       </c>
-      <c r="B2" s="3" t="n">
+      <c r="B2" s="8" t="n">
         <f aca="false">AVERAGE(Sheet1!$H$2:$H$67)</f>
         <v>18.0151515151515</v>
       </c>
@@ -3156,7 +3185,7 @@
       <c r="A3" s="0" t="s">
         <v>217</v>
       </c>
-      <c r="B3" s="3" t="n">
+      <c r="B3" s="8" t="n">
         <f aca="false">MEDIAN(Sheet1!$H$2:$H$67)</f>
         <v>12</v>
       </c>
@@ -3165,7 +3194,7 @@
       <c r="A4" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="B4" s="3" t="n">
+      <c r="B4" s="8" t="n">
         <f aca="false">STDEV(Sheet1!$H$2:$H$67)</f>
         <v>22.2119111665115</v>
       </c>

</xml_diff>

<commit_message>
starting 1TH and 2TH
</commit_message>
<xml_diff>
--- a/documentation/books.xlsx
+++ b/documentation/books.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="218">
   <si>
     <t xml:space="preserve">bible</t>
   </si>
@@ -530,6 +530,9 @@
   </si>
   <si>
     <t xml:space="preserve">1 Tesalonicenses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*</t>
   </si>
   <si>
     <t xml:space="preserve">1 Thessalonians</t>
@@ -946,13 +949,17 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1050,8 +1057,8 @@
   </sheetPr>
   <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G31" activeCellId="0" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2960,7 +2967,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="n">
         <v>51</v>
       </c>
@@ -2976,14 +2983,14 @@
       <c r="E53" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="F53" s="0" t="n">
-        <v>0</v>
+      <c r="F53" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="G53" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="I53" s="0" t="n">
         <v>5</v>
@@ -2992,7 +2999,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="n">
         <v>52</v>
       </c>
@@ -3003,19 +3010,19 @@
         <v>53</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E54" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="F54" s="0" t="n">
-        <v>0</v>
+      <c r="F54" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H54" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="I54" s="0" t="n">
         <v>3</v>
@@ -3035,7 +3042,7 @@
         <v>54</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E55" s="0" t="s">
         <v>131</v>
@@ -3044,10 +3051,10 @@
         <v>1</v>
       </c>
       <c r="G55" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H55" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I55" s="0" t="n">
         <v>6</v>
@@ -3073,7 +3080,7 @@
         <v>55</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E56" s="0" t="s">
         <v>131</v>
@@ -3082,10 +3089,10 @@
         <v>1</v>
       </c>
       <c r="G56" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H56" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="I56" s="0" t="n">
         <v>4</v>
@@ -3111,7 +3118,7 @@
         <v>56</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E57" s="0" t="s">
         <v>131</v>
@@ -3120,10 +3127,10 @@
         <v>1</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H57" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I57" s="0" t="n">
         <v>3</v>
@@ -3149,7 +3156,7 @@
         <v>57</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E58" s="0" t="s">
         <v>131</v>
@@ -3158,10 +3165,10 @@
         <v>1</v>
       </c>
       <c r="G58" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H58" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I58" s="0" t="n">
         <v>1</v>
@@ -3181,7 +3188,7 @@
         <v>58</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E59" s="0" t="s">
         <v>131</v>
@@ -3190,10 +3197,10 @@
         <v>1</v>
       </c>
       <c r="G59" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="H59" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="I59" s="0" t="n">
         <v>13</v>
@@ -3219,7 +3226,7 @@
         <v>59</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E60" s="0" t="s">
         <v>131</v>
@@ -3228,10 +3235,10 @@
         <v>1</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="H60" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="I60" s="0" t="n">
         <v>5</v>
@@ -3251,7 +3258,7 @@
         <v>60</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E61" s="0" t="s">
         <v>131</v>
@@ -3260,10 +3267,10 @@
         <v>1</v>
       </c>
       <c r="G61" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H61" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="I61" s="0" t="n">
         <v>5</v>
@@ -3289,7 +3296,7 @@
         <v>61</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E62" s="0" t="s">
         <v>131</v>
@@ -3298,10 +3305,10 @@
         <v>1</v>
       </c>
       <c r="G62" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="H62" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="I62" s="0" t="n">
         <v>3</v>
@@ -3321,7 +3328,7 @@
         <v>62</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E63" s="0" t="s">
         <v>131</v>
@@ -3330,10 +3337,10 @@
         <v>1</v>
       </c>
       <c r="G63" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="H63" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="I63" s="0" t="n">
         <v>5</v>
@@ -3353,7 +3360,7 @@
         <v>63</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E64" s="0" t="s">
         <v>131</v>
@@ -3362,10 +3369,10 @@
         <v>1</v>
       </c>
       <c r="G64" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="H64" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="I64" s="0" t="n">
         <v>1</v>
@@ -3385,7 +3392,7 @@
         <v>64</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E65" s="0" t="s">
         <v>131</v>
@@ -3394,10 +3401,10 @@
         <v>1</v>
       </c>
       <c r="G65" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="H65" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="I65" s="0" t="n">
         <v>1</v>
@@ -3417,7 +3424,7 @@
         <v>65</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E66" s="0" t="s">
         <v>131</v>
@@ -3426,10 +3433,10 @@
         <v>1</v>
       </c>
       <c r="G66" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="H66" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="I66" s="0" t="n">
         <v>1</v>
@@ -3455,7 +3462,7 @@
         <v>66</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E67" s="0" t="s">
         <v>131</v>
@@ -3464,10 +3471,10 @@
         <v>1</v>
       </c>
       <c r="G67" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="H67" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="I67" s="0" t="n">
         <v>22</v>
@@ -3498,7 +3505,7 @@
         <v>67</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F69" s="0" t="n">
         <v>51</v>
@@ -3512,7 +3519,7 @@
         <v>68</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="F70" s="0" t="n">
         <v>0.772727272727273</v>
@@ -3526,7 +3533,7 @@
         <v>69</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="F71" s="0" t="n">
         <v>14</v>

</xml_diff>

<commit_message>
Capítulos 1, 2 y 3 de TH2 corregidos
</commit_message>
<xml_diff>
--- a/documentation/books.xlsx
+++ b/documentation/books.xlsx
@@ -1057,8 +1057,8 @@
   </sheetPr>
   <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G31" activeCellId="0" sqref="G31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3500,7 +3500,7 @@
         <v>1189</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="n">
         <v>67</v>
       </c>
@@ -3508,13 +3508,15 @@
         <v>215</v>
       </c>
       <c r="F69" s="0" t="n">
-        <v>51</v>
+        <f aca="false">SUMIF(F2:F67,1)</f>
+        <v>52</v>
       </c>
       <c r="I69" s="0" t="n">
-        <v>925</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">SUMIF(F2:F67,1,I2:I67)</f>
+        <v>872</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="n">
         <v>68</v>
       </c>
@@ -3522,10 +3524,12 @@
         <v>216</v>
       </c>
       <c r="F70" s="0" t="n">
-        <v>0.772727272727273</v>
+        <f aca="false">F69/F68</f>
+        <v>0.787878787878788</v>
       </c>
       <c r="I70" s="0" t="n">
-        <v>0.777964676198486</v>
+        <f aca="false">I69/I68</f>
+        <v>0.733389402859546</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Introduciendo 1TH y 2TH en archivo principal
</commit_message>
<xml_diff>
--- a/documentation/books.xlsx
+++ b/documentation/books.xlsx
@@ -10,6 +10,10 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$L$71</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$L$71</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -20,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="218">
   <si>
     <t xml:space="preserve">bible</t>
   </si>
@@ -262,6 +266,9 @@
     <t xml:space="preserve">Isaías</t>
   </si>
   <si>
+    <t xml:space="preserve">*</t>
+  </si>
+  <si>
     <t xml:space="preserve">Isaiah</t>
   </si>
   <si>
@@ -530,9 +537,6 @@
   </si>
   <si>
     <t xml:space="preserve">1 Tesalonicenses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*</t>
   </si>
   <si>
     <t xml:space="preserve">1 Thessalonians</t>
@@ -1050,6 +1054,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -1057,8 +1065,8 @@
   </sheetPr>
   <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1883,7 +1891,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
         <v>22</v>
       </c>
@@ -1899,20 +1907,20 @@
       <c r="E24" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F24" s="0" t="n">
-        <v>0</v>
+      <c r="F24" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I24" s="0" t="n">
         <v>66</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1926,7 +1934,7 @@
         <v>24</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E25" s="0" t="s">
         <v>12</v>
@@ -1935,16 +1943,16 @@
         <v>1</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I25" s="0" t="n">
         <v>52</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K25" s="0" t="n">
         <v>32.1848747980769</v>
@@ -1964,7 +1972,7 @@
         <v>25</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E26" s="0" t="s">
         <v>12</v>
@@ -1973,10 +1981,10 @@
         <v>1</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I26" s="0" t="n">
         <v>5</v>
@@ -2002,7 +2010,7 @@
         <v>26</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E27" s="0" t="s">
         <v>12</v>
@@ -2011,16 +2019,16 @@
         <v>1</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I27" s="0" t="n">
         <v>48</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K27" s="0" t="n">
         <v>31.595325428</v>
@@ -2040,7 +2048,7 @@
         <v>27</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E28" s="0" t="s">
         <v>12</v>
@@ -2049,16 +2057,16 @@
         <v>1</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I28" s="0" t="n">
         <v>12</v>
       </c>
       <c r="J28" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K28" s="0" t="n">
         <v>29.8858247285714</v>
@@ -2078,7 +2086,7 @@
         <v>28</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E29" s="0" t="s">
         <v>12</v>
@@ -2087,16 +2095,16 @@
         <v>1</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I29" s="0" t="n">
         <v>14</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K29" s="0" t="n">
         <v>31.9816348666667</v>
@@ -2116,7 +2124,7 @@
         <v>29</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E30" s="0" t="s">
         <v>12</v>
@@ -2125,16 +2133,16 @@
         <v>1</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I30" s="0" t="n">
         <v>3</v>
       </c>
       <c r="J30" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K30" s="0" t="n">
         <v>31.8192574909091</v>
@@ -2154,7 +2162,7 @@
         <v>30</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E31" s="0" t="s">
         <v>12</v>
@@ -2163,16 +2171,16 @@
         <v>1</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="I31" s="0" t="n">
         <v>9</v>
       </c>
       <c r="J31" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K31" s="0" t="n">
         <v>31.806583025</v>
@@ -2192,7 +2200,7 @@
         <v>31</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E32" s="0" t="s">
         <v>12</v>
@@ -2201,16 +2209,16 @@
         <v>1</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="I32" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J32" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K32" s="0" t="n">
         <v>31.6097782777778</v>
@@ -2230,7 +2238,7 @@
         <v>32</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E33" s="0" t="s">
         <v>12</v>
@@ -2239,10 +2247,10 @@
         <v>1</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I33" s="0" t="n">
         <v>4</v>
@@ -2268,7 +2276,7 @@
         <v>33</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E34" s="0" t="s">
         <v>12</v>
@@ -2277,16 +2285,16 @@
         <v>1</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I34" s="0" t="n">
         <v>7</v>
       </c>
       <c r="J34" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K34" s="0" t="n">
         <v>32.0309007307692</v>
@@ -2306,7 +2314,7 @@
         <v>34</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E35" s="0" t="s">
         <v>12</v>
@@ -2315,16 +2323,16 @@
         <v>1</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I35" s="0" t="n">
         <v>3</v>
       </c>
       <c r="J35" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K35" s="0" t="n">
         <v>30.02499748</v>
@@ -2344,7 +2352,7 @@
         <v>35</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E36" s="0" t="s">
         <v>12</v>
@@ -2353,16 +2361,16 @@
         <v>1</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="I36" s="0" t="n">
         <v>3</v>
       </c>
       <c r="J36" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K36" s="0" t="n">
         <v>31.8736</v>
@@ -2382,7 +2390,7 @@
         <v>36</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E37" s="0" t="s">
         <v>12</v>
@@ -2391,16 +2399,16 @@
         <v>1</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I37" s="0" t="n">
         <v>3</v>
       </c>
       <c r="J37" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K37" s="0" t="n">
         <v>30.59335771</v>
@@ -2420,7 +2428,7 @@
         <v>37</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E38" s="0" t="s">
         <v>12</v>
@@ -2429,16 +2437,16 @@
         <v>1</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I38" s="0" t="n">
         <v>2</v>
       </c>
       <c r="J38" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K38" s="0" t="n">
         <v>30.7391216</v>
@@ -2458,7 +2466,7 @@
         <v>38</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E39" s="0" t="s">
         <v>12</v>
@@ -2467,16 +2475,16 @@
         <v>1</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I39" s="0" t="n">
         <v>14</v>
       </c>
       <c r="J39" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K39" s="0" t="n">
         <v>32.4826757615385</v>
@@ -2496,7 +2504,7 @@
         <v>39</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E40" s="0" t="s">
         <v>12</v>
@@ -2505,16 +2513,16 @@
         <v>1</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I40" s="0" t="n">
         <v>4</v>
       </c>
       <c r="J40" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K40" s="0" t="n">
         <v>31.2363364</v>
@@ -2534,25 +2542,25 @@
         <v>40</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F41" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="I41" s="0" t="n">
         <v>28</v>
       </c>
       <c r="J41" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="K41" s="0" t="n">
         <v>32.3827941576923</v>
@@ -2572,25 +2580,25 @@
         <v>41</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F42" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="I42" s="0" t="n">
         <v>16</v>
       </c>
       <c r="J42" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="K42" s="0" t="n">
         <v>32.2966465</v>
@@ -2610,25 +2618,25 @@
         <v>42</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F43" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I43" s="0" t="n">
         <v>24</v>
       </c>
       <c r="J43" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="K43" s="0" t="n">
         <v>32.5674360666667</v>
@@ -2648,25 +2656,25 @@
         <v>43</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F44" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="I44" s="0" t="n">
         <v>21</v>
       </c>
       <c r="J44" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="K44" s="0" t="n">
         <v>32.0573878642857</v>
@@ -2686,25 +2694,25 @@
         <v>44</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F45" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H45" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I45" s="0" t="n">
         <v>28</v>
       </c>
       <c r="J45" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="K45" s="0" t="n">
         <v>34.1376530137931</v>
@@ -2724,25 +2732,25 @@
         <v>45</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F46" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="I46" s="0" t="n">
         <v>16</v>
       </c>
       <c r="J46" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K46" s="0" t="n">
         <v>36.4487784833333</v>
@@ -2762,25 +2770,25 @@
         <v>46</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F47" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="I47" s="0" t="n">
         <v>16</v>
       </c>
       <c r="J47" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K47" s="0" t="n">
         <v>33.6480191111111</v>
@@ -2800,25 +2808,25 @@
         <v>47</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F48" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I48" s="0" t="n">
         <v>13</v>
       </c>
       <c r="J48" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K48" s="0" t="n">
         <v>35.8952308111111</v>
@@ -2838,25 +2846,25 @@
         <v>48</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F49" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="I49" s="0" t="n">
         <v>6</v>
       </c>
       <c r="J49" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K49" s="0" t="n">
         <v>31.0277102</v>
@@ -2876,25 +2884,25 @@
         <v>49</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F50" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G50" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H50" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="I50" s="0" t="n">
         <v>6</v>
       </c>
       <c r="J50" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2908,25 +2916,25 @@
         <v>50</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F51" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="I51" s="0" t="n">
         <v>4</v>
       </c>
       <c r="J51" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K51" s="0" t="n">
         <v>37.7649163</v>
@@ -2946,25 +2954,25 @@
         <v>51</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F52" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="I52" s="0" t="n">
         <v>4</v>
       </c>
       <c r="J52" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2978,13 +2986,13 @@
         <v>52</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>170</v>
+        <v>132</v>
+      </c>
+      <c r="F53" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="G53" s="0" t="s">
         <v>171</v>
@@ -2996,7 +3004,7 @@
         <v>5</v>
       </c>
       <c r="J53" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3013,10 +3021,10 @@
         <v>173</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>170</v>
+        <v>132</v>
+      </c>
+      <c r="F54" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="G54" s="0" t="s">
         <v>174</v>
@@ -3028,7 +3036,7 @@
         <v>3</v>
       </c>
       <c r="J54" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3045,7 +3053,7 @@
         <v>176</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F55" s="0" t="n">
         <v>1</v>
@@ -3060,7 +3068,7 @@
         <v>6</v>
       </c>
       <c r="J55" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K55" s="0" t="n">
         <v>39.77852525</v>
@@ -3083,7 +3091,7 @@
         <v>179</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F56" s="0" t="n">
         <v>1</v>
@@ -3098,7 +3106,7 @@
         <v>4</v>
       </c>
       <c r="J56" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K56" s="0" t="n">
         <v>38.8302656777778</v>
@@ -3121,7 +3129,7 @@
         <v>182</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F57" s="0" t="n">
         <v>1</v>
@@ -3136,7 +3144,7 @@
         <v>3</v>
       </c>
       <c r="J57" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K57" s="0" t="n">
         <v>35.240117</v>
@@ -3159,7 +3167,7 @@
         <v>185</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F58" s="0" t="n">
         <v>1</v>
@@ -3174,7 +3182,7 @@
         <v>1</v>
       </c>
       <c r="J58" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3191,7 +3199,7 @@
         <v>188</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F59" s="0" t="n">
         <v>1</v>
@@ -3206,7 +3214,7 @@
         <v>13</v>
       </c>
       <c r="J59" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K59" s="0" t="n">
         <v>30.4690138857143</v>
@@ -3229,7 +3237,7 @@
         <v>191</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F60" s="0" t="n">
         <v>1</v>
@@ -3244,7 +3252,7 @@
         <v>5</v>
       </c>
       <c r="J60" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3261,7 +3269,7 @@
         <v>194</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F61" s="0" t="n">
         <v>1</v>
@@ -3276,7 +3284,7 @@
         <v>5</v>
       </c>
       <c r="J61" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K61" s="0" t="n">
         <v>36.0484985</v>
@@ -3299,7 +3307,7 @@
         <v>197</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F62" s="0" t="n">
         <v>1</v>
@@ -3314,7 +3322,7 @@
         <v>3</v>
       </c>
       <c r="J62" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3331,7 +3339,7 @@
         <v>200</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F63" s="0" t="n">
         <v>1</v>
@@ -3346,7 +3354,7 @@
         <v>5</v>
       </c>
       <c r="J63" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3363,7 +3371,7 @@
         <v>203</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F64" s="0" t="n">
         <v>1</v>
@@ -3378,7 +3386,7 @@
         <v>1</v>
       </c>
       <c r="J64" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3395,7 +3403,7 @@
         <v>206</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F65" s="0" t="n">
         <v>1</v>
@@ -3410,7 +3418,7 @@
         <v>1</v>
       </c>
       <c r="J65" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3427,7 +3435,7 @@
         <v>209</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F66" s="0" t="n">
         <v>1</v>
@@ -3442,7 +3450,7 @@
         <v>1</v>
       </c>
       <c r="J66" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K66" s="0" t="n">
         <v>26.820553</v>
@@ -3465,7 +3473,7 @@
         <v>212</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F67" s="0" t="n">
         <v>1</v>
@@ -3480,7 +3488,7 @@
         <v>22</v>
       </c>
       <c r="J67" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K67" s="0" t="n">
         <v>34.9747663545455</v>
@@ -3509,11 +3517,11 @@
       </c>
       <c r="F69" s="0" t="n">
         <f aca="false">SUMIF(F2:F67,1)</f>
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I69" s="0" t="n">
         <f aca="false">SUMIF(F2:F67,1,I2:I67)</f>
-        <v>872</v>
+        <v>880</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3525,11 +3533,11 @@
       </c>
       <c r="F70" s="0" t="n">
         <f aca="false">F69/F68</f>
-        <v>0.787878787878788</v>
+        <v>0.818181818181818</v>
       </c>
       <c r="I70" s="0" t="n">
         <f aca="false">I69/I68</f>
-        <v>0.733389402859546</v>
+        <v>0.740117746005046</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3547,6 +3555,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="B1:L71"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3554,5 +3563,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
nueva información sobre localización de otras entidades
</commit_message>
<xml_diff>
--- a/documentation/books.xlsx
+++ b/documentation/books.xlsx
@@ -10,10 +10,6 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$L$71</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$L$71</definedName>
-  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -684,8 +680,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
   <fonts count="16">
     <font>
@@ -953,7 +950,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -964,6 +961,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1054,10 +1055,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -1065,8 +1062,8 @@
   </sheetPr>
   <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1179,10 +1176,10 @@
         <v>15</v>
       </c>
       <c r="K3" s="0" t="n">
-        <v>30.3698383</v>
+        <v>30.4699688976191</v>
       </c>
       <c r="L3" s="0" t="n">
-        <v>33.7367165076923</v>
+        <v>33.8432804079365</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1508,6 +1505,12 @@
       <c r="J12" s="0" t="s">
         <v>15</v>
       </c>
+      <c r="K12" s="0" t="n">
+        <v>31.8670741222222</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <v>35.1852309356481</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
@@ -1783,10 +1786,10 @@
         <v>69</v>
       </c>
       <c r="K20" s="0" t="n">
-        <v>30.9268848483871</v>
+        <v>30.9532842802083</v>
       </c>
       <c r="L20" s="0" t="n">
-        <v>35.4378564161291</v>
+        <v>35.4313175003472</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1955,10 +1958,10 @@
         <v>87</v>
       </c>
       <c r="K25" s="0" t="n">
-        <v>32.1848747980769</v>
+        <v>32.340919558642</v>
       </c>
       <c r="L25" s="0" t="n">
-        <v>35.5432907730769</v>
+        <v>35.4158287465021</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1993,10 +1996,10 @@
         <v>69</v>
       </c>
       <c r="K26" s="0" t="n">
-        <v>31.71697948</v>
+        <v>31.7260940111112</v>
       </c>
       <c r="L26" s="0" t="n">
-        <v>35.19855448</v>
+        <v>35.2035639185185</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2031,10 +2034,10 @@
         <v>87</v>
       </c>
       <c r="K27" s="0" t="n">
-        <v>31.595325428</v>
+        <v>31.5987830993464</v>
       </c>
       <c r="L27" s="0" t="n">
-        <v>35.46590773</v>
+        <v>35.4612548551198</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2069,10 +2072,10 @@
         <v>87</v>
       </c>
       <c r="K28" s="0" t="n">
-        <v>29.8858247285714</v>
+        <v>30.0115475244445</v>
       </c>
       <c r="L28" s="0" t="n">
-        <v>37.0924016</v>
+        <v>36.9681489007407</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2145,10 +2148,10 @@
         <v>87</v>
       </c>
       <c r="K30" s="0" t="n">
-        <v>31.8192574909091</v>
+        <v>31.8152915888889</v>
       </c>
       <c r="L30" s="0" t="n">
-        <v>33.2236226818182</v>
+        <v>33.3907050509259</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2183,10 +2186,10 @@
         <v>87</v>
       </c>
       <c r="K31" s="0" t="n">
-        <v>31.806583025</v>
+        <v>31.8051863706667</v>
       </c>
       <c r="L31" s="0" t="n">
-        <v>35.0503126916667</v>
+        <v>35.0574446284444</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2221,10 +2224,10 @@
         <v>87</v>
       </c>
       <c r="K32" s="0" t="n">
-        <v>31.6097782777778</v>
+        <v>31.6259671166667</v>
       </c>
       <c r="L32" s="0" t="n">
-        <v>35.2083436222222</v>
+        <v>35.2103703711111</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2297,10 +2300,10 @@
         <v>87</v>
       </c>
       <c r="K34" s="0" t="n">
-        <v>32.0309007307692</v>
+        <v>32.0123840119048</v>
       </c>
       <c r="L34" s="0" t="n">
-        <v>36.3155120384615</v>
+        <v>36.2378762579365</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2411,10 +2414,10 @@
         <v>87</v>
       </c>
       <c r="K37" s="0" t="n">
-        <v>30.59335771</v>
+        <v>30.7004767060606</v>
       </c>
       <c r="L37" s="0" t="n">
-        <v>35.38185619</v>
+        <v>35.3679248191919</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2487,10 +2490,10 @@
         <v>87</v>
       </c>
       <c r="K39" s="0" t="n">
-        <v>32.4826757615385</v>
+        <v>32.4563420913581</v>
       </c>
       <c r="L39" s="0" t="n">
-        <v>34.6678293</v>
+        <v>34.6885989967078</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2563,10 +2566,10 @@
         <v>135</v>
       </c>
       <c r="K41" s="0" t="n">
-        <v>32.3827941576923</v>
+        <v>32.3601598061729</v>
       </c>
       <c r="L41" s="0" t="n">
-        <v>35.0697941153846</v>
+        <v>35.0756762263374</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2715,10 +2718,10 @@
         <v>135</v>
       </c>
       <c r="K45" s="0" t="n">
-        <v>34.1376530137931</v>
+        <v>34.1861673694915</v>
       </c>
       <c r="L45" s="0" t="n">
-        <v>30.4890043758621</v>
+        <v>30.4976653186441</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2753,10 +2756,10 @@
         <v>151</v>
       </c>
       <c r="K46" s="0" t="n">
-        <v>36.4487784833333</v>
+        <v>35.780619652381</v>
       </c>
       <c r="L46" s="0" t="n">
-        <v>22.6268803166667</v>
+        <v>24.4271275730159</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2975,7 +2978,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="n">
         <v>51</v>
       </c>
@@ -2991,7 +2994,7 @@
       <c r="E53" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="F53" s="2" t="n">
+      <c r="F53" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G53" s="0" t="s">
@@ -3006,8 +3009,14 @@
       <c r="J53" s="0" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K53" s="0" t="n">
+        <v>38.033930725</v>
+      </c>
+      <c r="L53" s="0" t="n">
+        <v>25.905193075</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="n">
         <v>52</v>
       </c>
@@ -3023,7 +3032,7 @@
       <c r="E54" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="F54" s="2" t="n">
+      <c r="F54" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G54" s="0" t="s">
@@ -3217,10 +3226,10 @@
         <v>151</v>
       </c>
       <c r="K59" s="0" t="n">
-        <v>30.4690138857143</v>
+        <v>30.6318454833334</v>
       </c>
       <c r="L59" s="0" t="n">
-        <v>31.6284801</v>
+        <v>32.0784964763889</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3287,10 +3296,10 @@
         <v>151</v>
       </c>
       <c r="K61" s="0" t="n">
-        <v>36.0484985</v>
+        <v>34.622887888889</v>
       </c>
       <c r="L61" s="0" t="n">
-        <v>39.2791095</v>
+        <v>37.9289433703703</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3324,6 +3333,12 @@
       <c r="J62" s="0" t="s">
         <v>151</v>
       </c>
+      <c r="K62" s="0" t="n">
+        <v>31.771666666667</v>
+      </c>
+      <c r="L62" s="0" t="n">
+        <v>35.228611111111</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="n">
@@ -3491,13 +3506,13 @@
         <v>83</v>
       </c>
       <c r="K67" s="0" t="n">
-        <v>34.9747663545455</v>
+        <v>34.7078413805556</v>
       </c>
       <c r="L67" s="0" t="n">
-        <v>33.3589254</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>33.5147325425926</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="n">
         <v>66</v>
       </c>
@@ -3531,16 +3546,18 @@
       <c r="E70" s="0" t="s">
         <v>216</v>
       </c>
-      <c r="F70" s="0" t="n">
+      <c r="F70" s="3" t="n">
         <f aca="false">F69/F68</f>
         <v>0.818181818181818</v>
       </c>
-      <c r="I70" s="0" t="n">
+      <c r="G70" s="3"/>
+      <c r="H70" s="3"/>
+      <c r="I70" s="3" t="n">
         <f aca="false">I69/I68</f>
         <v>0.740117746005046</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="n">
         <v>69</v>
       </c>
@@ -3548,14 +3565,15 @@
         <v>217</v>
       </c>
       <c r="F71" s="0" t="n">
-        <v>14</v>
+        <f aca="false">F68*(1-F70)</f>
+        <v>12</v>
       </c>
       <c r="I71" s="0" t="n">
-        <v>392</v>
+        <f aca="false">I68*(1-I70)</f>
+        <v>309</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:L71"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3563,6 +3581,5 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New information about location of genres
</commit_message>
<xml_diff>
--- a/documentation/books.xlsx
+++ b/documentation/books.xlsx
@@ -427,7 +427,7 @@
     <t xml:space="preserve">MAT</t>
   </si>
   <si>
-    <t xml:space="preserve">Gospel</t>
+    <t xml:space="preserve">gospel</t>
   </si>
   <si>
     <t xml:space="preserve">Marcos</t>
@@ -1062,8 +1062,8 @@
   </sheetPr>
   <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A53" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J67" activeCellId="0" sqref="J67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2572,7 +2572,7 @@
         <v>35.0756762263374</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
         <v>40</v>
       </c>
@@ -2610,7 +2610,7 @@
         <v>34.6599276315789</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
         <v>41</v>
       </c>
@@ -2648,7 +2648,7 @@
         <v>35.6911872666667</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="n">
         <v>42</v>
       </c>
@@ -2686,7 +2686,7 @@
         <v>35.3856338214286</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="n">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
capítulo 1 de 2 Reyes
</commit_message>
<xml_diff>
--- a/documentation/books.xlsx
+++ b/documentation/books.xlsx
@@ -10,6 +10,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$L$71</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="218">
   <si>
     <t xml:space="preserve">bible</t>
   </si>
@@ -158,6 +161,9 @@
   </si>
   <si>
     <t xml:space="preserve">2 Reyes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*</t>
   </si>
   <si>
     <t xml:space="preserve">2 Kings</t>
@@ -790,6 +796,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -797,8 +807,8 @@
   </sheetPr>
   <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F51" activeCellId="0" sqref="F51"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1263,14 +1273,14 @@
       <c r="E13" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="0" t="n">
-        <v>0</v>
+      <c r="F13" s="0" t="s">
+        <v>46</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I13" s="0" t="n">
         <v>25</v>
@@ -1290,7 +1300,7 @@
         <v>13</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E14" s="0" t="s">
         <v>12</v>
@@ -1299,10 +1309,10 @@
         <v>0</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I14" s="0" t="n">
         <v>29</v>
@@ -1322,7 +1332,7 @@
         <v>14</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E15" s="0" t="s">
         <v>12</v>
@@ -1331,10 +1341,10 @@
         <v>0</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I15" s="0" t="n">
         <v>36</v>
@@ -1354,7 +1364,7 @@
         <v>15</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E16" s="0" t="s">
         <v>12</v>
@@ -1363,10 +1373,10 @@
         <v>1</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I16" s="0" t="n">
         <v>10</v>
@@ -1392,7 +1402,7 @@
         <v>16</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E17" s="0" t="s">
         <v>12</v>
@@ -1401,10 +1411,10 @@
         <v>1</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I17" s="0" t="n">
         <v>13</v>
@@ -1430,7 +1440,7 @@
         <v>17</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E18" s="0" t="s">
         <v>12</v>
@@ -1439,10 +1449,10 @@
         <v>0</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I18" s="0" t="n">
         <v>10</v>
@@ -1462,7 +1472,7 @@
         <v>18</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E19" s="0" t="s">
         <v>12</v>
@@ -1471,16 +1481,16 @@
         <v>1</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I19" s="0" t="n">
         <v>42</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K19" s="0" t="n">
         <v>19.865082</v>
@@ -1500,7 +1510,7 @@
         <v>19</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E20" s="0" t="s">
         <v>12</v>
@@ -1509,16 +1519,16 @@
         <v>1</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I20" s="0" t="n">
         <v>150</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K20" s="0" t="n">
         <v>30.9532842802083</v>
@@ -1538,7 +1548,7 @@
         <v>20</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E21" s="0" t="s">
         <v>12</v>
@@ -1547,16 +1557,16 @@
         <v>0</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I21" s="0" t="n">
         <v>31</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1570,7 +1580,7 @@
         <v>21</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E22" s="0" t="s">
         <v>12</v>
@@ -1579,16 +1589,16 @@
         <v>1</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I22" s="0" t="n">
         <v>12</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K22" s="0" t="n">
         <v>32.0003456666667</v>
@@ -1608,7 +1618,7 @@
         <v>22</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E23" s="0" t="s">
         <v>12</v>
@@ -1617,16 +1627,16 @@
         <v>0</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I23" s="0" t="n">
         <v>8</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1640,7 +1650,7 @@
         <v>23</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E24" s="0" t="s">
         <v>12</v>
@@ -1649,16 +1659,16 @@
         <v>1</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I24" s="0" t="n">
         <v>66</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K24" s="0" t="n">
         <v>31.558286685034</v>
@@ -1678,7 +1688,7 @@
         <v>24</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E25" s="0" t="s">
         <v>12</v>
@@ -1687,16 +1697,16 @@
         <v>1</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I25" s="0" t="n">
         <v>52</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K25" s="0" t="n">
         <v>32.340919558642</v>
@@ -1716,7 +1726,7 @@
         <v>25</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E26" s="0" t="s">
         <v>12</v>
@@ -1725,16 +1735,16 @@
         <v>1</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I26" s="0" t="n">
         <v>5</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K26" s="0" t="n">
         <v>31.7260940111112</v>
@@ -1754,7 +1764,7 @@
         <v>26</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E27" s="0" t="s">
         <v>12</v>
@@ -1763,16 +1773,16 @@
         <v>1</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I27" s="0" t="n">
         <v>48</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K27" s="0" t="n">
         <v>31.5987830993464</v>
@@ -1792,7 +1802,7 @@
         <v>27</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E28" s="0" t="s">
         <v>12</v>
@@ -1801,16 +1811,16 @@
         <v>1</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I28" s="0" t="n">
         <v>12</v>
       </c>
       <c r="J28" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K28" s="0" t="n">
         <v>30.0115475244445</v>
@@ -1830,7 +1840,7 @@
         <v>28</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E29" s="0" t="s">
         <v>12</v>
@@ -1839,16 +1849,16 @@
         <v>1</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I29" s="0" t="n">
         <v>14</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K29" s="0" t="n">
         <v>31.9816348666667</v>
@@ -1868,7 +1878,7 @@
         <v>29</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E30" s="0" t="s">
         <v>12</v>
@@ -1877,16 +1887,16 @@
         <v>1</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I30" s="0" t="n">
         <v>3</v>
       </c>
       <c r="J30" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K30" s="0" t="n">
         <v>31.8152915888889</v>
@@ -1906,7 +1916,7 @@
         <v>30</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E31" s="0" t="s">
         <v>12</v>
@@ -1915,16 +1925,16 @@
         <v>1</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="I31" s="0" t="n">
         <v>9</v>
       </c>
       <c r="J31" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K31" s="0" t="n">
         <v>31.8051863706667</v>
@@ -1944,7 +1954,7 @@
         <v>31</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E32" s="0" t="s">
         <v>12</v>
@@ -1953,16 +1963,16 @@
         <v>1</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="I32" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J32" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K32" s="0" t="n">
         <v>31.6259671166667</v>
@@ -1982,7 +1992,7 @@
         <v>32</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E33" s="0" t="s">
         <v>12</v>
@@ -1991,10 +2001,10 @@
         <v>1</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I33" s="0" t="n">
         <v>4</v>
@@ -2020,7 +2030,7 @@
         <v>33</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E34" s="0" t="s">
         <v>12</v>
@@ -2029,16 +2039,16 @@
         <v>1</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I34" s="0" t="n">
         <v>7</v>
       </c>
       <c r="J34" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K34" s="0" t="n">
         <v>32.0123840119048</v>
@@ -2058,7 +2068,7 @@
         <v>34</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E35" s="0" t="s">
         <v>12</v>
@@ -2067,16 +2077,16 @@
         <v>1</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I35" s="0" t="n">
         <v>3</v>
       </c>
       <c r="J35" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K35" s="0" t="n">
         <v>30.02499748</v>
@@ -2096,7 +2106,7 @@
         <v>35</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E36" s="0" t="s">
         <v>12</v>
@@ -2105,16 +2115,16 @@
         <v>1</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="I36" s="0" t="n">
         <v>3</v>
       </c>
       <c r="J36" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K36" s="0" t="n">
         <v>31.8736</v>
@@ -2134,7 +2144,7 @@
         <v>36</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E37" s="0" t="s">
         <v>12</v>
@@ -2143,16 +2153,16 @@
         <v>1</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I37" s="0" t="n">
         <v>3</v>
       </c>
       <c r="J37" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K37" s="0" t="n">
         <v>30.7004767060606</v>
@@ -2172,7 +2182,7 @@
         <v>37</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E38" s="0" t="s">
         <v>12</v>
@@ -2181,16 +2191,16 @@
         <v>1</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I38" s="0" t="n">
         <v>2</v>
       </c>
       <c r="J38" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K38" s="0" t="n">
         <v>30.7391216</v>
@@ -2210,7 +2220,7 @@
         <v>38</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E39" s="0" t="s">
         <v>12</v>
@@ -2219,16 +2229,16 @@
         <v>1</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I39" s="0" t="n">
         <v>14</v>
       </c>
       <c r="J39" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K39" s="0" t="n">
         <v>32.4563420913581</v>
@@ -2248,7 +2258,7 @@
         <v>39</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E40" s="0" t="s">
         <v>12</v>
@@ -2257,16 +2267,16 @@
         <v>1</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I40" s="0" t="n">
         <v>4</v>
       </c>
       <c r="J40" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K40" s="0" t="n">
         <v>31.2363364</v>
@@ -2286,25 +2296,25 @@
         <v>40</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F41" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="I41" s="0" t="n">
         <v>28</v>
       </c>
       <c r="J41" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="K41" s="0" t="n">
         <v>32.3601598061729</v>
@@ -2324,25 +2334,25 @@
         <v>41</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F42" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="I42" s="0" t="n">
         <v>16</v>
       </c>
       <c r="J42" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="K42" s="0" t="n">
         <v>32.2966465</v>
@@ -2362,25 +2372,25 @@
         <v>42</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F43" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I43" s="0" t="n">
         <v>24</v>
       </c>
       <c r="J43" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="K43" s="0" t="n">
         <v>32.5674360666667</v>
@@ -2400,25 +2410,25 @@
         <v>43</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F44" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="I44" s="0" t="n">
         <v>21</v>
       </c>
       <c r="J44" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="K44" s="0" t="n">
         <v>32.0573878642857</v>
@@ -2438,25 +2448,25 @@
         <v>44</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F45" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H45" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I45" s="0" t="n">
         <v>28</v>
       </c>
       <c r="J45" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="K45" s="0" t="n">
         <v>34.1861673694915</v>
@@ -2476,25 +2486,25 @@
         <v>45</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F46" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="I46" s="0" t="n">
         <v>16</v>
       </c>
       <c r="J46" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K46" s="0" t="n">
         <v>35.780619652381</v>
@@ -2514,25 +2524,25 @@
         <v>46</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F47" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="I47" s="0" t="n">
         <v>16</v>
       </c>
       <c r="J47" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K47" s="0" t="n">
         <v>33.6480191111111</v>
@@ -2552,25 +2562,25 @@
         <v>47</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F48" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I48" s="0" t="n">
         <v>13</v>
       </c>
       <c r="J48" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K48" s="0" t="n">
         <v>35.8952308111111</v>
@@ -2590,25 +2600,25 @@
         <v>48</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F49" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="I49" s="0" t="n">
         <v>6</v>
       </c>
       <c r="J49" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K49" s="0" t="n">
         <v>31.0277102</v>
@@ -2617,7 +2627,7 @@
         <v>37.2690598</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="n">
         <v>48</v>
       </c>
@@ -2628,25 +2638,31 @@
         <v>49</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="F50" s="2" t="n">
+        <v>132</v>
+      </c>
+      <c r="F50" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G50" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H50" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="I50" s="0" t="n">
         <v>6</v>
       </c>
       <c r="J50" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
+      </c>
+      <c r="K50" s="0" t="n">
+        <v>34.9773208333333</v>
+      </c>
+      <c r="L50" s="0" t="n">
+        <v>25.5316944</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2660,25 +2676,25 @@
         <v>50</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F51" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="I51" s="0" t="n">
         <v>4</v>
       </c>
       <c r="J51" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K51" s="0" t="n">
         <v>37.7649163</v>
@@ -2698,25 +2714,25 @@
         <v>51</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F52" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="I52" s="0" t="n">
         <v>4</v>
       </c>
       <c r="J52" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2730,25 +2746,25 @@
         <v>52</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F53" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G53" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="I53" s="0" t="n">
         <v>5</v>
       </c>
       <c r="J53" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K53" s="0" t="n">
         <v>38.033930725</v>
@@ -2768,25 +2784,25 @@
         <v>53</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F54" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H54" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="I54" s="0" t="n">
         <v>3</v>
       </c>
       <c r="J54" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2800,25 +2816,25 @@
         <v>54</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F55" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G55" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H55" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I55" s="0" t="n">
         <v>6</v>
       </c>
       <c r="J55" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K55" s="0" t="n">
         <v>39.77852525</v>
@@ -2838,25 +2854,25 @@
         <v>55</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F56" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G56" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H56" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="I56" s="0" t="n">
         <v>4</v>
       </c>
       <c r="J56" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K56" s="0" t="n">
         <v>38.8302656777778</v>
@@ -2876,25 +2892,25 @@
         <v>56</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F57" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H57" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I57" s="0" t="n">
         <v>3</v>
       </c>
       <c r="J57" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K57" s="0" t="n">
         <v>35.240117</v>
@@ -2914,25 +2930,25 @@
         <v>57</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F58" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G58" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H58" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I58" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J58" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2946,25 +2962,25 @@
         <v>58</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F59" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G59" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="H59" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="I59" s="0" t="n">
         <v>13</v>
       </c>
       <c r="J59" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K59" s="0" t="n">
         <v>30.6318454833334</v>
@@ -2984,25 +3000,25 @@
         <v>59</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F60" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="H60" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="I60" s="0" t="n">
         <v>5</v>
       </c>
       <c r="J60" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3016,25 +3032,25 @@
         <v>60</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F61" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G61" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H61" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="I61" s="0" t="n">
         <v>5</v>
       </c>
       <c r="J61" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K61" s="0" t="n">
         <v>34.622887888889</v>
@@ -3054,25 +3070,25 @@
         <v>61</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F62" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G62" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="H62" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="I62" s="0" t="n">
         <v>3</v>
       </c>
       <c r="J62" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K62" s="0" t="n">
         <v>31.771666666667</v>
@@ -3092,25 +3108,25 @@
         <v>62</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F63" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G63" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="H63" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="I63" s="0" t="n">
         <v>5</v>
       </c>
       <c r="J63" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3124,25 +3140,25 @@
         <v>63</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F64" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G64" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="H64" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="I64" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J64" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3156,25 +3172,25 @@
         <v>64</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F65" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G65" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="H65" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="I65" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J65" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3188,25 +3204,25 @@
         <v>65</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F66" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G66" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="H66" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="I66" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J66" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K66" s="0" t="n">
         <v>26.820553</v>
@@ -3226,25 +3242,25 @@
         <v>66</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F67" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G67" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="H67" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="I67" s="0" t="n">
         <v>22</v>
       </c>
       <c r="J67" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K67" s="0" t="n">
         <v>34.7078413805556</v>
@@ -3253,7 +3269,7 @@
         <v>33.5147325425926</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="n">
         <v>66</v>
       </c>
@@ -3268,14 +3284,16 @@
       <c r="A69" s="1" t="n">
         <v>67</v>
       </c>
-      <c r="E69" s="0" t="s">
-        <v>214</v>
-      </c>
-      <c r="F69" s="0" t="n">
+      <c r="E69" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F69" s="2" t="n">
         <f aca="false">SUMIF(F2:F67,1)</f>
         <v>56</v>
       </c>
-      <c r="I69" s="0" t="n">
+      <c r="G69" s="2"/>
+      <c r="H69" s="2"/>
+      <c r="I69" s="2" t="n">
         <f aca="false">SUMIF(F2:F67,1,I2:I67)</f>
         <v>952</v>
       </c>
@@ -3284,8 +3302,8 @@
       <c r="A70" s="1" t="n">
         <v>68</v>
       </c>
-      <c r="E70" s="0" t="s">
-        <v>215</v>
+      <c r="E70" s="2" t="s">
+        <v>216</v>
       </c>
       <c r="F70" s="3" t="n">
         <f aca="false">F69/F68</f>
@@ -3302,19 +3320,22 @@
       <c r="A71" s="1" t="n">
         <v>69</v>
       </c>
-      <c r="E71" s="0" t="s">
-        <v>216</v>
-      </c>
-      <c r="F71" s="0" t="n">
+      <c r="E71" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="F71" s="2" t="n">
         <f aca="false">F68*(1-F70)</f>
         <v>10</v>
       </c>
-      <c r="I71" s="0" t="n">
+      <c r="G71" s="2"/>
+      <c r="H71" s="2"/>
+      <c r="I71" s="2" t="n">
         <f aca="false">I68*(1-I70)</f>
         <v>237</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="B1:L71"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3322,5 +3343,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
2 Reyes terminado, bravo!
</commit_message>
<xml_diff>
--- a/documentation/books.xlsx
+++ b/documentation/books.xlsx
@@ -163,52 +163,52 @@
     <t xml:space="preserve">2 Reyes</t>
   </si>
   <si>
+    <t xml:space="preserve">2 Kings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2KI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Crónicas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Chronicles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1CH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Crónicas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Chronicles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2CH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Esdras</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ezra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EZR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nehemías</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nehemiah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ester</t>
+  </si>
+  <si>
     <t xml:space="preserve">*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 Kings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2KI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 Crónicas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 Chronicles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1CH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 Crónicas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 Chronicles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2CH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Esdras</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ezra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EZR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nehemías</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nehemiah</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NEH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ester</t>
   </si>
   <si>
     <t xml:space="preserve">Esther</t>
@@ -807,8 +807,8 @@
   </sheetPr>
   <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F31" activeCellId="0" sqref="F31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G28" activeCellId="0" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1273,14 +1273,14 @@
       <c r="E13" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="F13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="G13" s="0" t="s">
+      <c r="H13" s="0" t="s">
         <v>47</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>48</v>
       </c>
       <c r="I13" s="0" t="n">
         <v>25</v>
@@ -1300,19 +1300,19 @@
         <v>13</v>
       </c>
       <c r="D14" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" s="0" t="s">
+      <c r="H14" s="0" t="s">
         <v>50</v>
-      </c>
-      <c r="H14" s="0" t="s">
-        <v>51</v>
       </c>
       <c r="I14" s="0" t="n">
         <v>29</v>
@@ -1332,19 +1332,19 @@
         <v>14</v>
       </c>
       <c r="D15" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="E15" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G15" s="0" t="s">
+      <c r="H15" s="0" t="s">
         <v>53</v>
-      </c>
-      <c r="H15" s="0" t="s">
-        <v>54</v>
       </c>
       <c r="I15" s="0" t="n">
         <v>36</v>
@@ -1364,19 +1364,19 @@
         <v>15</v>
       </c>
       <c r="D16" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G16" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="E16" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G16" s="0" t="s">
+      <c r="H16" s="0" t="s">
         <v>56</v>
-      </c>
-      <c r="H16" s="0" t="s">
-        <v>57</v>
       </c>
       <c r="I16" s="0" t="n">
         <v>10</v>
@@ -1402,19 +1402,19 @@
         <v>16</v>
       </c>
       <c r="D17" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="E17" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G17" s="0" t="s">
+      <c r="H17" s="0" t="s">
         <v>59</v>
-      </c>
-      <c r="H17" s="0" t="s">
-        <v>60</v>
       </c>
       <c r="I17" s="0" t="n">
         <v>13</v>
@@ -1440,13 +1440,13 @@
         <v>17</v>
       </c>
       <c r="D18" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="0" t="s">
         <v>61</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="0" t="n">
-        <v>0</v>
       </c>
       <c r="G18" s="0" t="s">
         <v>62</v>
@@ -3289,13 +3289,13 @@
       </c>
       <c r="F69" s="2" t="n">
         <f aca="false">SUMIF(F2:F67,1)</f>
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
       <c r="I69" s="2" t="n">
         <f aca="false">SUMIF(F2:F67,1,I2:I67)</f>
-        <v>952</v>
+        <v>977</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3307,13 +3307,13 @@
       </c>
       <c r="F70" s="3" t="n">
         <f aca="false">F69/F68</f>
-        <v>0.848484848484848</v>
+        <v>0.863636363636364</v>
       </c>
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
       <c r="I70" s="3" t="n">
         <f aca="false">I69/I68</f>
-        <v>0.80067283431455</v>
+        <v>0.821698906644239</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3325,13 +3325,13 @@
       </c>
       <c r="F71" s="2" t="n">
         <f aca="false">F68*(1-F70)</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
       <c r="I71" s="2" t="n">
         <f aca="false">I68*(1-I70)</f>
-        <v>237</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Empezando Ester, capítulo 1 corregido
</commit_message>
<xml_diff>
--- a/documentation/books.xlsx
+++ b/documentation/books.xlsx
@@ -31,7 +31,7 @@
     <t xml:space="preserve">libro</t>
   </si>
   <si>
-    <t xml:space="preserve">testamen</t>
+    <t xml:space="preserve">testament</t>
   </si>
   <si>
     <t xml:space="preserve">encoded</t>
@@ -801,7 +801,7 @@
   <dimension ref="A1:L71"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Terminando números, empezando proverbios
</commit_message>
<xml_diff>
--- a/documentation/books.xlsx
+++ b/documentation/books.xlsx
@@ -94,148 +94,148 @@
     <t xml:space="preserve">Números</t>
   </si>
   <si>
+    <t xml:space="preserve">Numbers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deuteronomio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deuteronomy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Josué</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joshua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jueces</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Judges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JDG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ruth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RUT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Samuel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1SA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Samuel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2SA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Reyes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Kings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1KI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Reyes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Kings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2KI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Crónicas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Chronicles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1CH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Crónicas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Chronicles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2CH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Esdras</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ezra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EZR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nehemías</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nehemiah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ester</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Esther</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Job</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wisdom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salmos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Psalms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lyric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proverbios</t>
+  </si>
+  <si>
     <t xml:space="preserve">*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NUM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deuteronomio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deuteronomy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Josué</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Joshua</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jueces</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Judges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JDG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rut</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ruth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RUT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 Samuel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1SA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 Samuel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2SA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 Reyes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 Kings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1KI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 Reyes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 Kings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2KI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 Crónicas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 Chronicles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1CH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 Crónicas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 Chronicles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2CH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Esdras</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ezra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EZR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nehemías</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nehemiah</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NEH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ester</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Esther</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Job</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JOB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wisdom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Salmos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Psalms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PSA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lyric</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proverbios</t>
   </si>
   <si>
     <t xml:space="preserve">Proverbs</t>
@@ -800,8 +800,8 @@
   </sheetPr>
   <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J18" activeCellId="0" sqref="J18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A42" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L63" activeCellId="0" sqref="L63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -974,20 +974,26 @@
       <c r="E5" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="F5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="H5" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>26</v>
       </c>
       <c r="I5" s="0" t="n">
         <v>36</v>
       </c>
       <c r="J5" s="0" t="s">
         <v>22</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>31.2216179928572</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>34.8414332857143</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1001,19 +1007,19 @@
         <v>5</v>
       </c>
       <c r="D6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" s="0" t="s">
+      <c r="H6" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>34</v>
@@ -1033,19 +1039,19 @@
         <v>6</v>
       </c>
       <c r="D7" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" s="0" t="s">
+      <c r="H7" s="0" t="s">
         <v>31</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>32</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>24</v>
@@ -1071,19 +1077,19 @@
         <v>7</v>
       </c>
       <c r="D8" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" s="0" t="s">
+      <c r="H8" s="0" t="s">
         <v>34</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>35</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>21</v>
@@ -1109,19 +1115,19 @@
         <v>8</v>
       </c>
       <c r="D9" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G9" s="0" t="s">
+      <c r="H9" s="0" t="s">
         <v>37</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>38</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>4</v>
@@ -1147,19 +1153,19 @@
         <v>9</v>
       </c>
       <c r="D10" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" s="0" t="s">
         <v>39</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>40</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>31</v>
@@ -1185,19 +1191,19 @@
         <v>10</v>
       </c>
       <c r="D11" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="0" t="s">
         <v>41</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>42</v>
       </c>
       <c r="I11" s="0" t="n">
         <v>24</v>
@@ -1223,19 +1229,19 @@
         <v>11</v>
       </c>
       <c r="D12" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G12" s="0" t="s">
+      <c r="H12" s="0" t="s">
         <v>44</v>
-      </c>
-      <c r="H12" s="0" t="s">
-        <v>45</v>
       </c>
       <c r="I12" s="0" t="n">
         <v>22</v>
@@ -1261,19 +1267,19 @@
         <v>12</v>
       </c>
       <c r="D13" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G13" s="0" t="s">
+      <c r="H13" s="0" t="s">
         <v>47</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>48</v>
       </c>
       <c r="I13" s="0" t="n">
         <v>25</v>
@@ -1299,19 +1305,19 @@
         <v>13</v>
       </c>
       <c r="D14" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" s="0" t="s">
+      <c r="H14" s="0" t="s">
         <v>50</v>
-      </c>
-      <c r="H14" s="0" t="s">
-        <v>51</v>
       </c>
       <c r="I14" s="0" t="n">
         <v>29</v>
@@ -1331,19 +1337,19 @@
         <v>14</v>
       </c>
       <c r="D15" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="E15" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G15" s="0" t="s">
+      <c r="H15" s="0" t="s">
         <v>53</v>
-      </c>
-      <c r="H15" s="0" t="s">
-        <v>54</v>
       </c>
       <c r="I15" s="0" t="n">
         <v>36</v>
@@ -1363,19 +1369,19 @@
         <v>15</v>
       </c>
       <c r="D16" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G16" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="E16" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G16" s="0" t="s">
+      <c r="H16" s="0" t="s">
         <v>56</v>
-      </c>
-      <c r="H16" s="0" t="s">
-        <v>57</v>
       </c>
       <c r="I16" s="0" t="n">
         <v>10</v>
@@ -1401,19 +1407,19 @@
         <v>16</v>
       </c>
       <c r="D17" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="E17" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G17" s="0" t="s">
+      <c r="H17" s="0" t="s">
         <v>59</v>
-      </c>
-      <c r="H17" s="0" t="s">
-        <v>60</v>
       </c>
       <c r="I17" s="0" t="n">
         <v>13</v>
@@ -1439,19 +1445,19 @@
         <v>17</v>
       </c>
       <c r="D18" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G18" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="E18" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G18" s="0" t="s">
+      <c r="H18" s="0" t="s">
         <v>62</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>63</v>
       </c>
       <c r="I18" s="0" t="n">
         <v>10</v>
@@ -1477,25 +1483,25 @@
         <v>18</v>
       </c>
       <c r="D19" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="H19" s="0" t="s">
         <v>64</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G19" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="H19" s="0" t="s">
-        <v>65</v>
       </c>
       <c r="I19" s="0" t="n">
         <v>42</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K19" s="0" t="n">
         <v>19.865082</v>
@@ -1515,25 +1521,25 @@
         <v>19</v>
       </c>
       <c r="D20" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G20" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="E20" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G20" s="0" t="s">
+      <c r="H20" s="0" t="s">
         <v>68</v>
-      </c>
-      <c r="H20" s="0" t="s">
-        <v>69</v>
       </c>
       <c r="I20" s="0" t="n">
         <v>150</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K20" s="0" t="n">
         <v>30.9532842802083</v>
@@ -1553,13 +1559,13 @@
         <v>20</v>
       </c>
       <c r="D21" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="0" t="s">
         <v>71</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F21" s="0" t="n">
-        <v>0</v>
       </c>
       <c r="G21" s="0" t="s">
         <v>72</v>
@@ -1571,7 +1577,7 @@
         <v>31</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1603,7 +1609,7 @@
         <v>12</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K22" s="0" t="n">
         <v>32.0003456666667</v>
@@ -1641,7 +1647,7 @@
         <v>8</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1749,7 +1755,7 @@
         <v>5</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K26" s="0" t="n">
         <v>31.7260940111112</v>
@@ -3294,13 +3300,13 @@
       </c>
       <c r="F69" s="2" t="n">
         <f aca="false">SUMIF(F2:F67,1)</f>
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
       <c r="I69" s="2" t="n">
         <f aca="false">SUMIF(F2:F67,1,I2:I67)</f>
-        <v>987</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3312,13 +3318,13 @@
       </c>
       <c r="F70" s="3" t="n">
         <f aca="false">F69/F68</f>
-        <v>0.878787878787879</v>
+        <v>0.893939393939394</v>
       </c>
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
       <c r="I70" s="3" t="n">
         <f aca="false">I69/I68</f>
-        <v>0.830109335576114</v>
+        <v>0.860386879730866</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3330,13 +3336,13 @@
       </c>
       <c r="F71" s="2" t="n">
         <f aca="false">F68*(1-F70)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
       <c r="I71" s="2" t="n">
         <f aca="false">I68*(1-I70)</f>
-        <v>202</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
terminando cantar de los cantares
</commit_message>
<xml_diff>
--- a/documentation/books.xlsx
+++ b/documentation/books.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="218">
   <si>
     <t xml:space="preserve">bible</t>
   </si>
@@ -169,6 +169,9 @@
     <t xml:space="preserve">1 Crónicas</t>
   </si>
   <si>
+    <t xml:space="preserve">*</t>
+  </si>
+  <si>
     <t xml:space="preserve">1 Chronicles</t>
   </si>
   <si>
@@ -251,9 +254,6 @@
   </si>
   <si>
     <t xml:space="preserve">Cantares</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*</t>
   </si>
   <si>
     <t xml:space="preserve">Song of Solomon</t>
@@ -800,8 +800,8 @@
   </sheetPr>
   <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A47" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K65" activeCellId="0" sqref="K65"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E57" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I71" activeCellId="0" sqref="I71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1316,14 +1316,14 @@
       <c r="E14" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="0" t="n">
-        <v>0</v>
+      <c r="F14" s="0" t="s">
+        <v>49</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I14" s="0" t="n">
         <v>29</v>
@@ -1343,19 +1343,19 @@
         <v>14</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E15" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="0" t="n">
-        <v>0</v>
+      <c r="F15" s="0" t="s">
+        <v>49</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I15" s="0" t="n">
         <v>36</v>
@@ -1375,7 +1375,7 @@
         <v>15</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E16" s="0" t="s">
         <v>12</v>
@@ -1384,10 +1384,10 @@
         <v>1</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I16" s="0" t="n">
         <v>10</v>
@@ -1413,7 +1413,7 @@
         <v>16</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E17" s="0" t="s">
         <v>12</v>
@@ -1422,10 +1422,10 @@
         <v>1</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I17" s="0" t="n">
         <v>13</v>
@@ -1451,7 +1451,7 @@
         <v>17</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E18" s="0" t="s">
         <v>12</v>
@@ -1460,10 +1460,10 @@
         <v>1</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I18" s="0" t="n">
         <v>10</v>
@@ -1489,7 +1489,7 @@
         <v>18</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E19" s="0" t="s">
         <v>12</v>
@@ -1498,16 +1498,16 @@
         <v>1</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I19" s="0" t="n">
         <v>42</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K19" s="0" t="n">
         <v>19.865082</v>
@@ -1527,7 +1527,7 @@
         <v>19</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E20" s="0" t="s">
         <v>12</v>
@@ -1536,16 +1536,16 @@
         <v>1</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I20" s="0" t="n">
         <v>150</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K20" s="0" t="n">
         <v>30.9532842802083</v>
@@ -1565,7 +1565,7 @@
         <v>20</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E21" s="0" t="s">
         <v>12</v>
@@ -1574,16 +1574,16 @@
         <v>1</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I21" s="0" t="n">
         <v>31</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K21" s="0" t="n">
         <v>29.9232731333333</v>
@@ -1603,7 +1603,7 @@
         <v>21</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E22" s="0" t="s">
         <v>12</v>
@@ -1612,16 +1612,16 @@
         <v>1</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I22" s="0" t="n">
         <v>12</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K22" s="0" t="n">
         <v>32.0003456666667</v>
@@ -1641,13 +1641,13 @@
         <v>22</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E23" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F23" s="0" t="s">
-        <v>77</v>
+      <c r="F23" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="G23" s="0" t="s">
         <v>78</v>
@@ -1659,7 +1659,13 @@
         <v>8</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
+      </c>
+      <c r="K23" s="0" t="n">
+        <v>32.2361352458334</v>
+      </c>
+      <c r="L23" s="0" t="n">
+        <v>35.5485861263889</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1767,7 +1773,7 @@
         <v>5</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K26" s="0" t="n">
         <v>31.7260940111112</v>
@@ -3298,7 +3304,7 @@
         <v>33.5147325425926</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="n">
         <v>66</v>
       </c>
@@ -3318,13 +3324,13 @@
       </c>
       <c r="F69" s="2" t="n">
         <f aca="false">SUMIF(F2:F67,1)</f>
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
       <c r="I69" s="2" t="n">
         <f aca="false">SUMIF(F2:F67,1,I2:I67)</f>
-        <v>1092</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3336,13 +3342,13 @@
       </c>
       <c r="F70" s="3" t="n">
         <f aca="false">F69/F68</f>
-        <v>0.939393939393939</v>
+        <v>0.954545454545455</v>
       </c>
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
       <c r="I70" s="3" t="n">
         <f aca="false">I69/I68</f>
-        <v>0.918418839360807</v>
+        <v>0.925147182506308</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3354,13 +3360,13 @@
       </c>
       <c r="F71" s="2" t="n">
         <f aca="false">F68*(1-F70)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
       <c r="I71" s="2" t="n">
         <f aca="false">I68*(1-I70)</f>
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Comenzando 1 crónicas, capítulo 1 corregido
</commit_message>
<xml_diff>
--- a/documentation/books.xlsx
+++ b/documentation/books.xlsx
@@ -800,8 +800,8 @@
   </sheetPr>
   <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E57" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I71" activeCellId="0" sqref="I71"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Capítulo 7 corregido (ohu)
</commit_message>
<xml_diff>
--- a/documentation/books.xlsx
+++ b/documentation/books.xlsx
@@ -965,8 +965,8 @@
   </sheetPr>
   <dimension ref="A1:M71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I68" activeCellId="0" sqref="I68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Finishing 1CH and 2CH
</commit_message>
<xml_diff>
--- a/documentation/books.xlsx
+++ b/documentation/books.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="269">
   <si>
     <t xml:space="preserve">bible</t>
   </si>
@@ -827,24 +827,14 @@
   </si>
   <si>
     <t xml:space="preserve">Rev</t>
-  </si>
-  <si>
-    <t xml:space="preserve">total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">proportion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">total falta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -926,21 +916,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -962,8 +944,8 @@
   </sheetPr>
   <dimension ref="A1:M71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A60" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B63" activeCellId="0" sqref="B63"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A57" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A71" activeCellId="0" sqref="68:71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1005,11 +987,11 @@
       <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
@@ -1050,7 +1032,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
@@ -1091,7 +1073,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
@@ -1132,7 +1114,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
@@ -1173,7 +1155,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
@@ -1214,7 +1196,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
@@ -1255,7 +1237,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
@@ -1296,7 +1278,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
@@ -1337,7 +1319,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
@@ -1378,7 +1360,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
@@ -1419,7 +1401,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
@@ -1460,7 +1442,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
@@ -1501,7 +1483,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
@@ -1532,11 +1514,17 @@
       <c r="J14" s="0" t="s">
         <v>16</v>
       </c>
+      <c r="K14" s="0" t="n">
+        <v>32.0105521231884</v>
+      </c>
+      <c r="L14" s="0" t="n">
+        <v>36.031745213285</v>
+      </c>
       <c r="M14" s="0" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>13</v>
       </c>
@@ -1567,11 +1555,17 @@
       <c r="J15" s="0" t="s">
         <v>16</v>
       </c>
+      <c r="K15" s="0" t="n">
+        <v>32.0012473111111</v>
+      </c>
+      <c r="L15" s="0" t="n">
+        <v>35.8507288237473</v>
+      </c>
       <c r="M15" s="0" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>14</v>
       </c>
@@ -1612,7 +1606,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>15</v>
       </c>
@@ -1653,7 +1647,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
         <v>16</v>
       </c>
@@ -1694,7 +1688,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <v>17</v>
       </c>
@@ -1735,7 +1729,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <v>18</v>
       </c>
@@ -1776,7 +1770,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
         <v>19</v>
       </c>
@@ -1817,7 +1811,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
         <v>20</v>
       </c>
@@ -1858,7 +1852,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
         <v>21</v>
       </c>
@@ -1899,7 +1893,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
         <v>22</v>
       </c>
@@ -1940,7 +1934,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
         <v>23</v>
       </c>
@@ -1981,7 +1975,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
         <v>24</v>
       </c>
@@ -2022,7 +2016,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
         <v>25</v>
       </c>
@@ -2063,7 +2057,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
         <v>26</v>
       </c>
@@ -2104,7 +2098,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
         <v>27</v>
       </c>
@@ -2145,7 +2139,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
         <v>28</v>
       </c>
@@ -2186,7 +2180,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
         <v>29</v>
       </c>
@@ -2227,7 +2221,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
         <v>30</v>
       </c>
@@ -2268,7 +2262,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
         <v>31</v>
       </c>
@@ -2309,7 +2303,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
         <v>32</v>
       </c>
@@ -2350,7 +2344,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
         <v>33</v>
       </c>
@@ -2391,7 +2385,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
         <v>34</v>
       </c>
@@ -2432,7 +2426,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
         <v>35</v>
       </c>
@@ -2473,7 +2467,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="n">
         <v>36</v>
       </c>
@@ -2514,7 +2508,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
         <v>37</v>
       </c>
@@ -2555,7 +2549,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
         <v>38</v>
       </c>
@@ -2596,7 +2590,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="n">
         <v>39</v>
       </c>
@@ -2637,7 +2631,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
         <v>40</v>
       </c>
@@ -2678,7 +2672,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
         <v>41</v>
       </c>
@@ -2710,16 +2704,16 @@
         <v>168</v>
       </c>
       <c r="K43" s="0" t="n">
-        <v>32.5674360666667</v>
+        <v>32.6406997192308</v>
       </c>
       <c r="L43" s="0" t="n">
-        <v>35.6911872666667</v>
+        <v>35.0272764423077</v>
       </c>
       <c r="M43" s="0" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="n">
         <v>42</v>
       </c>
@@ -2760,7 +2754,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="n">
         <v>43</v>
       </c>
@@ -2801,7 +2795,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="n">
         <v>44</v>
       </c>
@@ -2842,7 +2836,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="n">
         <v>45</v>
       </c>
@@ -2883,7 +2877,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="n">
         <v>46</v>
       </c>
@@ -2924,7 +2918,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="n">
         <v>47</v>
       </c>
@@ -2965,7 +2959,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="n">
         <v>48</v>
       </c>
@@ -3006,7 +3000,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="n">
         <v>49</v>
       </c>
@@ -3047,7 +3041,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="n">
         <v>50</v>
       </c>
@@ -3088,7 +3082,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="n">
         <v>51</v>
       </c>
@@ -3129,7 +3123,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="n">
         <v>52</v>
       </c>
@@ -3164,7 +3158,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="n">
         <v>53</v>
       </c>
@@ -3205,7 +3199,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="n">
         <v>54</v>
       </c>
@@ -3246,7 +3240,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="n">
         <v>55</v>
       </c>
@@ -3287,7 +3281,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="n">
         <v>56</v>
       </c>
@@ -3322,7 +3316,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="n">
         <v>57</v>
       </c>
@@ -3363,7 +3357,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="n">
         <v>58</v>
       </c>
@@ -3398,7 +3392,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="n">
         <v>59</v>
       </c>
@@ -3439,7 +3433,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="n">
         <v>60</v>
       </c>
@@ -3480,7 +3474,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="n">
         <v>61</v>
       </c>
@@ -3515,7 +3509,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="n">
         <v>62</v>
       </c>
@@ -3550,7 +3544,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="n">
         <v>63</v>
       </c>
@@ -3585,7 +3579,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="n">
         <v>64</v>
       </c>
@@ -3626,7 +3620,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="n">
         <v>65</v>
       </c>
@@ -3668,69 +3662,16 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="1" t="n">
-        <v>66</v>
-      </c>
-      <c r="F68" s="0" t="n">
-        <v>66</v>
-      </c>
-      <c r="I68" s="0" t="n">
-        <v>1189</v>
-      </c>
+      <c r="A68" s="1"/>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="1" t="n">
-        <v>67</v>
-      </c>
-      <c r="E69" s="0" t="s">
-        <v>269</v>
-      </c>
-      <c r="F69" s="2" t="n">
-        <f aca="false">SUMIF(F2:F67,1)</f>
-        <v>66</v>
-      </c>
-      <c r="G69" s="2"/>
-      <c r="H69" s="2"/>
-      <c r="I69" s="2" t="n">
-        <f aca="false">SUMIF(F2:F67,1,I2:I67)</f>
-        <v>1189</v>
-      </c>
+      <c r="A69" s="1"/>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="1" t="n">
-        <v>68</v>
-      </c>
-      <c r="E70" s="0" t="s">
-        <v>270</v>
-      </c>
-      <c r="F70" s="3" t="n">
-        <f aca="false">F69/F68</f>
-        <v>1</v>
-      </c>
-      <c r="G70" s="3"/>
-      <c r="H70" s="3"/>
-      <c r="I70" s="3" t="n">
-        <f aca="false">I69/I68</f>
-        <v>1</v>
-      </c>
+      <c r="A70" s="1"/>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="1" t="n">
-        <v>69</v>
-      </c>
-      <c r="E71" s="0" t="s">
-        <v>271</v>
-      </c>
-      <c r="F71" s="2" t="n">
-        <f aca="false">F68*(1-F70)</f>
-        <v>0</v>
-      </c>
-      <c r="G71" s="2"/>
-      <c r="H71" s="2"/>
-      <c r="I71" s="2" t="n">
-        <f aca="false">I68*(1-I70)</f>
-        <v>0</v>
-      </c>
+      <c r="A71" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
adding John to the entire Bible file
</commit_message>
<xml_diff>
--- a/documentation/books.xlsx
+++ b/documentation/books.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$N$67</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$O$67</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$O$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$N$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$B$1:$M$67</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -1177,11 +1177,11 @@
   </sheetPr>
   <dimension ref="A1:O71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A39" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N44" activeCellId="0" sqref="N44"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G48" activeCellId="0" sqref="G48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
@@ -3168,7 +3168,9 @@
       <c r="N44" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="O44" s="4"/>
+      <c r="O44" s="4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="n">
@@ -4186,7 +4188,7 @@
       <c r="A71" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:N67"/>
+  <autoFilter ref="B1:O67"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
starting annotation of the psalms
</commit_message>
<xml_diff>
--- a/documentation/books.xlsx
+++ b/documentation/books.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$O$67</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$N$67</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$N$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$O$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$B$1:$M$67</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="338">
   <si>
     <t xml:space="preserve">bible</t>
   </si>
@@ -349,6 +349,9 @@
   </si>
   <si>
     <t xml:space="preserve">Q41064</t>
+  </si>
+  <si>
+    <t xml:space="preserve">next</t>
   </si>
   <si>
     <t xml:space="preserve">Proverbios</t>
@@ -1177,11 +1180,11 @@
   </sheetPr>
   <dimension ref="A1:O71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G48" activeCellId="0" sqref="G48"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O21" activeCellId="0" sqref="O21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
@@ -2084,7 +2087,9 @@
       <c r="N20" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="O20" s="4"/>
+      <c r="O20" s="4" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="n">
@@ -2097,7 +2102,7 @@
         <v>20</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>15</v>
@@ -2106,10 +2111,10 @@
         <v>1</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I21" s="3" t="n">
         <v>31</v>
@@ -2124,10 +2129,10 @@
         <v>33.6192164666667</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="N21" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O21" s="4"/>
     </row>
@@ -2142,7 +2147,7 @@
         <v>21</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>15</v>
@@ -2151,10 +2156,10 @@
         <v>1</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I22" s="3" t="n">
         <v>12</v>
@@ -2169,10 +2174,10 @@
         <v>35.228163</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="N22" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="O22" s="4"/>
     </row>
@@ -2187,7 +2192,7 @@
         <v>22</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>15</v>
@@ -2196,10 +2201,10 @@
         <v>1</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I23" s="3" t="n">
         <v>8</v>
@@ -2214,10 +2219,10 @@
         <v>35.5485861263889</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="N23" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O23" s="4" t="n">
         <v>1</v>
@@ -2234,7 +2239,7 @@
         <v>23</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>15</v>
@@ -2243,16 +2248,16 @@
         <v>1</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I24" s="3" t="n">
         <v>66</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="K24" s="3" t="n">
         <v>31.558286685034</v>
@@ -2261,10 +2266,10 @@
         <v>36.2484380798186</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="N24" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="O24" s="4"/>
     </row>
@@ -2279,7 +2284,7 @@
         <v>24</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>15</v>
@@ -2288,16 +2293,16 @@
         <v>1</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I25" s="3" t="n">
         <v>52</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K25" s="3" t="n">
         <v>32.340919558642</v>
@@ -2306,10 +2311,10 @@
         <v>35.4158287465021</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="N25" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="O25" s="4"/>
     </row>
@@ -2324,7 +2329,7 @@
         <v>25</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>15</v>
@@ -2333,10 +2338,10 @@
         <v>1</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="I26" s="3" t="n">
         <v>5</v>
@@ -2351,10 +2356,10 @@
         <v>35.2035639185185</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="N26" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="O26" s="4"/>
     </row>
@@ -2369,7 +2374,7 @@
         <v>26</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>15</v>
@@ -2378,16 +2383,16 @@
         <v>1</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="I27" s="3" t="n">
         <v>48</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K27" s="3" t="n">
         <v>31.5987830993464</v>
@@ -2396,10 +2401,10 @@
         <v>35.4612548551198</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="N27" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="O27" s="4"/>
     </row>
@@ -2414,7 +2419,7 @@
         <v>27</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>15</v>
@@ -2423,16 +2428,16 @@
         <v>1</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I28" s="3" t="n">
         <v>12</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K28" s="3" t="n">
         <v>30.0115475244445</v>
@@ -2441,10 +2446,10 @@
         <v>36.9681489007407</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="N28" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="O28" s="4"/>
     </row>
@@ -2459,7 +2464,7 @@
         <v>28</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>15</v>
@@ -2468,16 +2473,16 @@
         <v>1</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I29" s="3" t="n">
         <v>14</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K29" s="3" t="n">
         <v>31.9816348666667</v>
@@ -2486,10 +2491,10 @@
         <v>35.2501034333333</v>
       </c>
       <c r="M29" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="N29" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="O29" s="4"/>
     </row>
@@ -2504,7 +2509,7 @@
         <v>29</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>15</v>
@@ -2513,16 +2518,16 @@
         <v>1</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="I30" s="3" t="n">
         <v>3</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K30" s="3" t="n">
         <v>31.8152915888889</v>
@@ -2531,10 +2536,10 @@
         <v>33.3907050509259</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="N30" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="O30" s="4"/>
     </row>
@@ -2549,7 +2554,7 @@
         <v>30</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>15</v>
@@ -2558,16 +2563,16 @@
         <v>1</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="I31" s="3" t="n">
         <v>9</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K31" s="3" t="n">
         <v>31.8051863706667</v>
@@ -2576,10 +2581,10 @@
         <v>35.0574446284444</v>
       </c>
       <c r="M31" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="N31" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="O31" s="4"/>
     </row>
@@ -2594,7 +2599,7 @@
         <v>31</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>15</v>
@@ -2603,16 +2608,16 @@
         <v>1</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="I32" s="3" t="n">
         <v>1</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K32" s="3" t="n">
         <v>31.6259671166667</v>
@@ -2621,10 +2626,10 @@
         <v>35.2103703711111</v>
       </c>
       <c r="M32" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="N32" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="O32" s="4"/>
     </row>
@@ -2639,7 +2644,7 @@
         <v>32</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>15</v>
@@ -2648,10 +2653,10 @@
         <v>1</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="I33" s="3" t="n">
         <v>4</v>
@@ -2666,10 +2671,10 @@
         <v>34.9298637666667</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="N33" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="O33" s="4"/>
     </row>
@@ -2684,7 +2689,7 @@
         <v>33</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>15</v>
@@ -2693,16 +2698,16 @@
         <v>1</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="I34" s="3" t="n">
         <v>7</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K34" s="3" t="n">
         <v>32.0123840119048</v>
@@ -2711,10 +2716,10 @@
         <v>36.2378762579365</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="N34" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="O34" s="4"/>
     </row>
@@ -2729,7 +2734,7 @@
         <v>34</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>15</v>
@@ -2738,16 +2743,16 @@
         <v>1</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I35" s="3" t="n">
         <v>3</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K35" s="3" t="n">
         <v>30.02499748</v>
@@ -2756,10 +2761,10 @@
         <v>33.51317685</v>
       </c>
       <c r="M35" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="N35" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="O35" s="4"/>
     </row>
@@ -2774,7 +2779,7 @@
         <v>35</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>15</v>
@@ -2783,16 +2788,16 @@
         <v>1</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="I36" s="3" t="n">
         <v>3</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K36" s="3" t="n">
         <v>31.8736</v>
@@ -2801,10 +2806,10 @@
         <v>35.749305</v>
       </c>
       <c r="M36" s="3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="N36" s="3" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="O36" s="4"/>
     </row>
@@ -2819,7 +2824,7 @@
         <v>36</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>15</v>
@@ -2828,16 +2833,16 @@
         <v>1</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="I37" s="3" t="n">
         <v>3</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K37" s="3" t="n">
         <v>30.7004767060606</v>
@@ -2846,10 +2851,10 @@
         <v>35.3679248191919</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="N37" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="O37" s="4"/>
     </row>
@@ -2864,7 +2869,7 @@
         <v>37</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>15</v>
@@ -2873,16 +2878,16 @@
         <v>1</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="I38" s="3" t="n">
         <v>2</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K38" s="3" t="n">
         <v>30.7391216</v>
@@ -2891,10 +2896,10 @@
         <v>34.1192041</v>
       </c>
       <c r="M38" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="N38" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="O38" s="4"/>
     </row>
@@ -2909,7 +2914,7 @@
         <v>38</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>15</v>
@@ -2918,16 +2923,16 @@
         <v>1</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="I39" s="3" t="n">
         <v>14</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K39" s="3" t="n">
         <v>32.4563420913581</v>
@@ -2936,10 +2941,10 @@
         <v>34.6885989967078</v>
       </c>
       <c r="M39" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="N39" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="O39" s="4"/>
     </row>
@@ -2954,7 +2959,7 @@
         <v>39</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>15</v>
@@ -2963,16 +2968,16 @@
         <v>1</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="I40" s="3" t="n">
         <v>4</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K40" s="3" t="n">
         <v>31.2363364</v>
@@ -2981,10 +2986,10 @@
         <v>34.9578466</v>
       </c>
       <c r="M40" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="N40" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="O40" s="4"/>
     </row>
@@ -2999,25 +3004,25 @@
         <v>40</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F41" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="I41" s="3" t="n">
         <v>28</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="K41" s="3" t="n">
         <v>32.3601598061729</v>
@@ -3026,10 +3031,10 @@
         <v>35.0756762263374</v>
       </c>
       <c r="M41" s="3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="N41" s="3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="O41" s="4" t="n">
         <v>1</v>
@@ -3046,25 +3051,25 @@
         <v>41</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F42" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="I42" s="3" t="n">
         <v>16</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="K42" s="3" t="n">
         <v>32.2966465</v>
@@ -3073,10 +3078,10 @@
         <v>34.6599276315789</v>
       </c>
       <c r="M42" s="3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="N42" s="3" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="O42" s="4"/>
     </row>
@@ -3091,25 +3096,25 @@
         <v>42</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F43" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="I43" s="3" t="n">
         <v>24</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="K43" s="3" t="n">
         <v>32.6406997192308</v>
@@ -3118,10 +3123,10 @@
         <v>35.0272764423077</v>
       </c>
       <c r="M43" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="N43" s="3" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="O43" s="4"/>
     </row>
@@ -3136,25 +3141,25 @@
         <v>43</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F44" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="I44" s="3" t="n">
         <v>21</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="K44" s="3" t="n">
         <v>32.0573878642857</v>
@@ -3163,10 +3168,10 @@
         <v>35.3856338214286</v>
       </c>
       <c r="M44" s="3" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="N44" s="3" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="O44" s="4" t="n">
         <v>1</v>
@@ -3183,25 +3188,25 @@
         <v>44</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F45" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="I45" s="3" t="n">
         <v>28</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="K45" s="3" t="n">
         <v>34.1861673694915</v>
@@ -3210,10 +3215,10 @@
         <v>30.4976653186441</v>
       </c>
       <c r="M45" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="N45" s="3" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="O45" s="4"/>
     </row>
@@ -3228,25 +3233,25 @@
         <v>45</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F46" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="I46" s="3" t="n">
         <v>16</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="K46" s="3" t="n">
         <v>35.780619652381</v>
@@ -3255,10 +3260,10 @@
         <v>24.4271275730159</v>
       </c>
       <c r="M46" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="N46" s="3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="O46" s="4"/>
     </row>
@@ -3273,25 +3278,25 @@
         <v>46</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F47" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="I47" s="3" t="n">
         <v>16</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="K47" s="3" t="n">
         <v>33.6480191111111</v>
@@ -3300,10 +3305,10 @@
         <v>31.5965783888889</v>
       </c>
       <c r="M47" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="N47" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="O47" s="4" t="n">
         <v>1</v>
@@ -3320,25 +3325,25 @@
         <v>47</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F48" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="I48" s="3" t="n">
         <v>13</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="K48" s="3" t="n">
         <v>35.8952308111111</v>
@@ -3347,12 +3352,14 @@
         <v>29.4401928555556</v>
       </c>
       <c r="M48" s="3" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N48" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="O48" s="4"/>
+        <v>244</v>
+      </c>
+      <c r="O48" s="4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="n">
@@ -3365,25 +3372,25 @@
         <v>48</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F49" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="I49" s="3" t="n">
         <v>6</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="K49" s="3" t="n">
         <v>31.0277102</v>
@@ -3392,10 +3399,10 @@
         <v>37.2690598</v>
       </c>
       <c r="M49" s="3" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="N49" s="3" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="O49" s="4"/>
     </row>
@@ -3410,25 +3417,25 @@
         <v>49</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F50" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="I50" s="3" t="n">
         <v>6</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="K50" s="3" t="n">
         <v>34.9773208333333</v>
@@ -3437,10 +3444,10 @@
         <v>25.5316944</v>
       </c>
       <c r="M50" s="3" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="N50" s="3" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="O50" s="4"/>
     </row>
@@ -3455,25 +3462,25 @@
         <v>50</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F51" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="I51" s="3" t="n">
         <v>4</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="K51" s="3" t="n">
         <v>37.7649163</v>
@@ -3482,10 +3489,10 @@
         <v>26.5137687</v>
       </c>
       <c r="M51" s="3" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="N51" s="3" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="O51" s="4"/>
     </row>
@@ -3500,25 +3507,25 @@
         <v>51</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F52" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="I52" s="3" t="n">
         <v>4</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="K52" s="3" t="n">
         <v>35.5407103</v>
@@ -3527,10 +3534,10 @@
         <v>35.7952667</v>
       </c>
       <c r="M52" s="3" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="N52" s="3" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="O52" s="4"/>
     </row>
@@ -3545,25 +3552,25 @@
         <v>52</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F53" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="I53" s="3" t="n">
         <v>5</v>
       </c>
       <c r="J53" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="K53" s="3" t="n">
         <v>38.033930725</v>
@@ -3572,10 +3579,10 @@
         <v>25.905193075</v>
       </c>
       <c r="M53" s="3" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="N53" s="3" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="O53" s="4"/>
     </row>
@@ -3590,31 +3597,31 @@
         <v>53</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F54" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="I54" s="3" t="n">
         <v>3</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="M54" s="3" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="N54" s="3" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="O54" s="4"/>
     </row>
@@ -3629,25 +3636,25 @@
         <v>54</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F55" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="I55" s="3" t="n">
         <v>6</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="K55" s="3" t="n">
         <v>39.77852525</v>
@@ -3656,10 +3663,10 @@
         <v>24.5566651</v>
       </c>
       <c r="M55" s="3" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="N55" s="3" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="O55" s="4"/>
     </row>
@@ -3674,25 +3681,25 @@
         <v>55</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F56" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="I56" s="3" t="n">
         <v>4</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="K56" s="3" t="n">
         <v>38.8302656777778</v>
@@ -3701,10 +3708,10 @@
         <v>27.4323937222222</v>
       </c>
       <c r="M56" s="3" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="N56" s="3" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="O56" s="4"/>
     </row>
@@ -3719,25 +3726,25 @@
         <v>56</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F57" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="I57" s="3" t="n">
         <v>3</v>
       </c>
       <c r="J57" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="K57" s="3" t="n">
         <v>35.240117</v>
@@ -3746,10 +3753,10 @@
         <v>24.8092691</v>
       </c>
       <c r="M57" s="3" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="N57" s="3" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="O57" s="4"/>
     </row>
@@ -3764,31 +3771,31 @@
         <v>57</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F58" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="I58" s="3" t="n">
         <v>1</v>
       </c>
       <c r="J58" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="M58" s="3" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="N58" s="3" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="O58" s="4"/>
     </row>
@@ -3803,25 +3810,25 @@
         <v>58</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F59" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="I59" s="3" t="n">
         <v>13</v>
       </c>
       <c r="J59" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="K59" s="3" t="n">
         <v>30.6318454833334</v>
@@ -3830,10 +3837,10 @@
         <v>32.0784964763889</v>
       </c>
       <c r="M59" s="3" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="N59" s="3" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="O59" s="4"/>
     </row>
@@ -3848,31 +3855,31 @@
         <v>59</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F60" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="I60" s="3" t="n">
         <v>5</v>
       </c>
       <c r="J60" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="M60" s="3" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="N60" s="3" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="O60" s="4"/>
     </row>
@@ -3887,25 +3894,25 @@
         <v>60</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F61" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="I61" s="3" t="n">
         <v>5</v>
       </c>
       <c r="J61" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="K61" s="3" t="n">
         <v>34.622887888889</v>
@@ -3914,10 +3921,10 @@
         <v>37.9289433703703</v>
       </c>
       <c r="M61" s="3" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="N61" s="3" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="O61" s="4"/>
     </row>
@@ -3932,25 +3939,25 @@
         <v>61</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F62" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="H62" s="3" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="I62" s="3" t="n">
         <v>3</v>
       </c>
       <c r="J62" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="K62" s="3" t="n">
         <v>31.771666666667</v>
@@ -3959,10 +3966,10 @@
         <v>35.228611111111</v>
       </c>
       <c r="M62" s="3" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="N62" s="3" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="O62" s="4"/>
     </row>
@@ -3977,31 +3984,31 @@
         <v>62</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F63" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="I63" s="3" t="n">
         <v>5</v>
       </c>
       <c r="J63" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="M63" s="3" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="N63" s="3" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="O63" s="4"/>
     </row>
@@ -4016,31 +4023,31 @@
         <v>63</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F64" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="I64" s="3" t="n">
         <v>1</v>
       </c>
       <c r="J64" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="M64" s="3" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="N64" s="3" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="O64" s="4"/>
     </row>
@@ -4055,31 +4062,31 @@
         <v>64</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F65" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="I65" s="3" t="n">
         <v>1</v>
       </c>
       <c r="J65" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="M65" s="3" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="N65" s="3" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="O65" s="4"/>
     </row>
@@ -4094,25 +4101,25 @@
         <v>65</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F66" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="I66" s="3" t="n">
         <v>1</v>
       </c>
       <c r="J66" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="K66" s="3" t="n">
         <v>26.820553</v>
@@ -4121,10 +4128,10 @@
         <v>30.802498</v>
       </c>
       <c r="M66" s="3" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="N66" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="O66" s="4"/>
     </row>
@@ -4139,25 +4146,25 @@
         <v>66</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F67" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="I67" s="3" t="n">
         <v>22</v>
       </c>
       <c r="J67" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="K67" s="3" t="n">
         <v>34.7078413805556</v>
@@ -4166,10 +4173,10 @@
         <v>33.5147325425926</v>
       </c>
       <c r="M67" s="3" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="N67" s="3" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="O67" s="4" t="n">
         <v>1</v>
@@ -4188,7 +4195,7 @@
       <c r="A71" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:O67"/>
+  <autoFilter ref="B1:N67"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
integrated in main file several prophetical books
</commit_message>
<xml_diff>
--- a/documentation/books.xlsx
+++ b/documentation/books.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$P$67</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$Q$67</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$Q$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$P$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$B$1:$O$67</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="341">
   <si>
     <t xml:space="preserve">bible</t>
   </si>
@@ -352,9 +352,6 @@
   </si>
   <si>
     <t xml:space="preserve">Q41064</t>
-  </si>
-  <si>
-    <t xml:space="preserve">next</t>
   </si>
   <si>
     <t xml:space="preserve">Proverbios</t>
@@ -1192,11 +1189,11 @@
   </sheetPr>
   <dimension ref="A1:Q71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E29" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L48" activeCellId="0" sqref="L48"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q10" activeCellId="0" sqref="Q10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
@@ -2130,7 +2127,9 @@
       <c r="P19" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="Q19" s="4"/>
+      <c r="Q19" s="4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="n">
@@ -2179,8 +2178,8 @@
       <c r="P20" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="Q20" s="4" t="s">
-        <v>109</v>
+      <c r="Q20" s="4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2194,7 +2193,7 @@
         <v>20</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>16</v>
@@ -2203,10 +2202,10 @@
         <v>1</v>
       </c>
       <c r="G21" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="H21" s="3" t="s">
         <v>111</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>112</v>
       </c>
       <c r="I21" s="3"/>
       <c r="J21" s="3" t="n">
@@ -2225,10 +2224,10 @@
         <v>33.6192164666667</v>
       </c>
       <c r="O21" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="P21" s="3" t="s">
         <v>113</v>
-      </c>
-      <c r="P21" s="3" t="s">
-        <v>114</v>
       </c>
       <c r="Q21" s="4"/>
     </row>
@@ -2243,7 +2242,7 @@
         <v>21</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>16</v>
@@ -2252,10 +2251,10 @@
         <v>1</v>
       </c>
       <c r="G22" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="H22" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>117</v>
       </c>
       <c r="I22" s="3"/>
       <c r="J22" s="3" t="n">
@@ -2274,10 +2273,10 @@
         <v>35.228163</v>
       </c>
       <c r="O22" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="P22" s="3" t="s">
         <v>118</v>
-      </c>
-      <c r="P22" s="3" t="s">
-        <v>119</v>
       </c>
       <c r="Q22" s="4"/>
     </row>
@@ -2292,7 +2291,7 @@
         <v>22</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>16</v>
@@ -2301,10 +2300,10 @@
         <v>1</v>
       </c>
       <c r="G23" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="H23" s="3" t="s">
         <v>121</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>122</v>
       </c>
       <c r="I23" s="3"/>
       <c r="J23" s="3" t="n">
@@ -2323,10 +2322,10 @@
         <v>35.5485861263889</v>
       </c>
       <c r="O23" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="P23" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="P23" s="3" t="s">
-        <v>124</v>
       </c>
       <c r="Q23" s="4" t="n">
         <v>1</v>
@@ -2343,7 +2342,7 @@
         <v>23</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>16</v>
@@ -2352,20 +2351,20 @@
         <v>1</v>
       </c>
       <c r="G24" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="H24" s="3" t="s">
         <v>126</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>127</v>
       </c>
       <c r="I24" s="3"/>
       <c r="J24" s="3" t="n">
         <v>66</v>
       </c>
       <c r="K24" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="L24" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="L24" s="3" t="s">
-        <v>129</v>
       </c>
       <c r="M24" s="3" t="n">
         <v>31.558286685034</v>
@@ -2374,10 +2373,10 @@
         <v>36.2484380798186</v>
       </c>
       <c r="O24" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="P24" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="P24" s="3" t="s">
-        <v>131</v>
       </c>
       <c r="Q24" s="4"/>
     </row>
@@ -2392,7 +2391,7 @@
         <v>24</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>16</v>
@@ -2401,20 +2400,20 @@
         <v>1</v>
       </c>
       <c r="G25" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="H25" s="3" t="s">
         <v>133</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>134</v>
       </c>
       <c r="I25" s="3"/>
       <c r="J25" s="3" t="n">
         <v>52</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M25" s="3" t="n">
         <v>32.340919558642</v>
@@ -2423,10 +2422,10 @@
         <v>35.4158287465021</v>
       </c>
       <c r="O25" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="P25" s="3" t="s">
         <v>136</v>
-      </c>
-      <c r="P25" s="3" t="s">
-        <v>137</v>
       </c>
       <c r="Q25" s="4"/>
     </row>
@@ -2441,7 +2440,7 @@
         <v>25</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>16</v>
@@ -2450,10 +2449,10 @@
         <v>1</v>
       </c>
       <c r="G26" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="H26" s="3" t="s">
         <v>139</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>140</v>
       </c>
       <c r="I26" s="3"/>
       <c r="J26" s="3" t="n">
@@ -2472,10 +2471,10 @@
         <v>35.2035639185185</v>
       </c>
       <c r="O26" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="P26" s="3" t="s">
         <v>141</v>
-      </c>
-      <c r="P26" s="3" t="s">
-        <v>142</v>
       </c>
       <c r="Q26" s="4"/>
     </row>
@@ -2490,7 +2489,7 @@
         <v>26</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>16</v>
@@ -2499,20 +2498,20 @@
         <v>1</v>
       </c>
       <c r="G27" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="H27" s="3" t="s">
         <v>144</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>145</v>
       </c>
       <c r="I27" s="3"/>
       <c r="J27" s="3" t="n">
         <v>48</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M27" s="3" t="n">
         <v>31.5987830993464</v>
@@ -2521,12 +2520,14 @@
         <v>35.4612548551198</v>
       </c>
       <c r="O27" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="P27" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="P27" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="Q27" s="4"/>
+      <c r="Q27" s="4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="n">
@@ -2539,7 +2540,7 @@
         <v>27</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>16</v>
@@ -2548,20 +2549,20 @@
         <v>1</v>
       </c>
       <c r="G28" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="H28" s="3" t="s">
         <v>148</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>149</v>
       </c>
       <c r="I28" s="3"/>
       <c r="J28" s="3" t="n">
         <v>12</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M28" s="3" t="n">
         <v>30.0115475244445</v>
@@ -2570,10 +2571,10 @@
         <v>36.9681489007407</v>
       </c>
       <c r="O28" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="P28" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="P28" s="3" t="s">
-        <v>151</v>
       </c>
       <c r="Q28" s="4"/>
     </row>
@@ -2588,7 +2589,7 @@
         <v>28</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>16</v>
@@ -2597,20 +2598,20 @@
         <v>1</v>
       </c>
       <c r="G29" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="H29" s="3" t="s">
         <v>153</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>154</v>
       </c>
       <c r="I29" s="3"/>
       <c r="J29" s="3" t="n">
         <v>14</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M29" s="3" t="n">
         <v>31.9816348666667</v>
@@ -2619,10 +2620,10 @@
         <v>35.2501034333333</v>
       </c>
       <c r="O29" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="P29" s="3" t="s">
         <v>155</v>
-      </c>
-      <c r="P29" s="3" t="s">
-        <v>156</v>
       </c>
       <c r="Q29" s="4"/>
     </row>
@@ -2637,7 +2638,7 @@
         <v>29</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>16</v>
@@ -2646,20 +2647,20 @@
         <v>1</v>
       </c>
       <c r="G30" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="H30" s="3" t="s">
         <v>157</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>158</v>
       </c>
       <c r="I30" s="3"/>
       <c r="J30" s="3" t="n">
         <v>3</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M30" s="3" t="n">
         <v>31.8152915888889</v>
@@ -2668,10 +2669,10 @@
         <v>33.3907050509259</v>
       </c>
       <c r="O30" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="P30" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="Q30" s="4"/>
     </row>
@@ -2686,7 +2687,7 @@
         <v>30</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>16</v>
@@ -2695,20 +2696,20 @@
         <v>1</v>
       </c>
       <c r="G31" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H31" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>162</v>
       </c>
       <c r="I31" s="3"/>
       <c r="J31" s="3" t="n">
         <v>9</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M31" s="3" t="n">
         <v>31.8051863706667</v>
@@ -2717,10 +2718,10 @@
         <v>35.0574446284444</v>
       </c>
       <c r="O31" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="P31" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q31" s="4"/>
     </row>
@@ -2735,7 +2736,7 @@
         <v>31</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>16</v>
@@ -2744,20 +2745,20 @@
         <v>1</v>
       </c>
       <c r="G32" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="H32" s="3" t="s">
         <v>165</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>166</v>
       </c>
       <c r="I32" s="3"/>
       <c r="J32" s="3" t="n">
         <v>1</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M32" s="3" t="n">
         <v>31.6259671166667</v>
@@ -2766,10 +2767,10 @@
         <v>35.2103703711111</v>
       </c>
       <c r="O32" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="P32" s="3" t="s">
         <v>167</v>
-      </c>
-      <c r="P32" s="3" t="s">
-        <v>168</v>
       </c>
       <c r="Q32" s="4"/>
     </row>
@@ -2784,7 +2785,7 @@
         <v>32</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>16</v>
@@ -2793,10 +2794,10 @@
         <v>1</v>
       </c>
       <c r="G33" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="H33" s="3" t="s">
         <v>170</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>171</v>
       </c>
       <c r="I33" s="3"/>
       <c r="J33" s="3" t="n">
@@ -2806,7 +2807,7 @@
         <v>19</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M33" s="3" t="n">
         <v>36.6525328333333</v>
@@ -2815,10 +2816,10 @@
         <v>34.9298637666667</v>
       </c>
       <c r="O33" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="P33" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="Q33" s="4"/>
     </row>
@@ -2833,7 +2834,7 @@
         <v>33</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>16</v>
@@ -2842,20 +2843,20 @@
         <v>1</v>
       </c>
       <c r="G34" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="H34" s="3" t="s">
         <v>175</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>176</v>
       </c>
       <c r="I34" s="3"/>
       <c r="J34" s="3" t="n">
         <v>7</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M34" s="3" t="n">
         <v>32.0123840119048</v>
@@ -2864,10 +2865,10 @@
         <v>36.2378762579365</v>
       </c>
       <c r="O34" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="P34" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="P34" s="3" t="s">
-        <v>178</v>
       </c>
       <c r="Q34" s="4"/>
     </row>
@@ -2882,7 +2883,7 @@
         <v>34</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>16</v>
@@ -2891,20 +2892,20 @@
         <v>1</v>
       </c>
       <c r="G35" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="H35" s="3" t="s">
         <v>180</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>181</v>
       </c>
       <c r="I35" s="3"/>
       <c r="J35" s="3" t="n">
         <v>3</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L35" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M35" s="3" t="n">
         <v>30.02499748</v>
@@ -2913,12 +2914,14 @@
         <v>33.51317685</v>
       </c>
       <c r="O35" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="P35" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="P35" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="Q35" s="4"/>
+      <c r="Q35" s="4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="n">
@@ -2931,7 +2934,7 @@
         <v>35</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>16</v>
@@ -2940,20 +2943,20 @@
         <v>1</v>
       </c>
       <c r="G36" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="H36" s="3" t="s">
         <v>185</v>
-      </c>
-      <c r="H36" s="3" t="s">
-        <v>186</v>
       </c>
       <c r="I36" s="3"/>
       <c r="J36" s="3" t="n">
         <v>3</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L36" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M36" s="3" t="n">
         <v>31.8736</v>
@@ -2962,12 +2965,14 @@
         <v>35.749305</v>
       </c>
       <c r="O36" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="P36" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="P36" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="Q36" s="4"/>
+      <c r="Q36" s="4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="n">
@@ -2980,7 +2985,7 @@
         <v>36</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>16</v>
@@ -2989,20 +2994,20 @@
         <v>1</v>
       </c>
       <c r="G37" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="H37" s="3" t="s">
         <v>190</v>
-      </c>
-      <c r="H37" s="3" t="s">
-        <v>191</v>
       </c>
       <c r="I37" s="3"/>
       <c r="J37" s="3" t="n">
         <v>3</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L37" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M37" s="3" t="n">
         <v>30.7004767060606</v>
@@ -3011,12 +3016,14 @@
         <v>35.3679248191919</v>
       </c>
       <c r="O37" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="P37" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="P37" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="Q37" s="4"/>
+      <c r="Q37" s="4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="n">
@@ -3029,7 +3036,7 @@
         <v>37</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>16</v>
@@ -3038,20 +3045,20 @@
         <v>1</v>
       </c>
       <c r="G38" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="H38" s="3" t="s">
         <v>195</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>196</v>
       </c>
       <c r="I38" s="3"/>
       <c r="J38" s="3" t="n">
         <v>2</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L38" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M38" s="3" t="n">
         <v>30.7391216</v>
@@ -3060,12 +3067,14 @@
         <v>34.1192041</v>
       </c>
       <c r="O38" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="P38" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="P38" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="Q38" s="4"/>
+      <c r="Q38" s="4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="n">
@@ -3078,7 +3087,7 @@
         <v>38</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>16</v>
@@ -3087,20 +3096,20 @@
         <v>1</v>
       </c>
       <c r="G39" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="H39" s="3" t="s">
         <v>200</v>
-      </c>
-      <c r="H39" s="3" t="s">
-        <v>201</v>
       </c>
       <c r="I39" s="3"/>
       <c r="J39" s="3" t="n">
         <v>14</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L39" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M39" s="3" t="n">
         <v>32.4563420913581</v>
@@ -3109,12 +3118,14 @@
         <v>34.6885989967078</v>
       </c>
       <c r="O39" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="P39" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="P39" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="Q39" s="4"/>
+      <c r="Q39" s="4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="n">
@@ -3127,7 +3138,7 @@
         <v>39</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>16</v>
@@ -3136,20 +3147,20 @@
         <v>1</v>
       </c>
       <c r="G40" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="H40" s="3" t="s">
         <v>205</v>
-      </c>
-      <c r="H40" s="3" t="s">
-        <v>206</v>
       </c>
       <c r="I40" s="3"/>
       <c r="J40" s="3" t="n">
         <v>4</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L40" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M40" s="3" t="n">
         <v>31.2363364</v>
@@ -3158,10 +3169,10 @@
         <v>34.9578466</v>
       </c>
       <c r="O40" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="P40" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="P40" s="3" t="s">
-        <v>208</v>
       </c>
       <c r="Q40" s="4"/>
     </row>
@@ -3176,29 +3187,29 @@
         <v>40</v>
       </c>
       <c r="D41" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="E41" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="F41" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G41" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="F41" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G41" s="3" t="s">
+      <c r="H41" s="3" t="s">
         <v>211</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>212</v>
       </c>
       <c r="I41" s="3"/>
       <c r="J41" s="3" t="n">
         <v>28</v>
       </c>
       <c r="K41" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="L41" s="3" t="s">
         <v>213</v>
-      </c>
-      <c r="L41" s="3" t="s">
-        <v>214</v>
       </c>
       <c r="M41" s="3" t="n">
         <v>32.3601598061729</v>
@@ -3207,10 +3218,10 @@
         <v>35.0756762263374</v>
       </c>
       <c r="O41" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="P41" s="3" t="s">
         <v>215</v>
-      </c>
-      <c r="P41" s="3" t="s">
-        <v>216</v>
       </c>
       <c r="Q41" s="4" t="n">
         <v>1</v>
@@ -3227,29 +3238,29 @@
         <v>41</v>
       </c>
       <c r="D42" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="F42" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G42" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="E42" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="F42" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G42" s="3" t="s">
+      <c r="H42" s="3" t="s">
         <v>218</v>
-      </c>
-      <c r="H42" s="3" t="s">
-        <v>219</v>
       </c>
       <c r="I42" s="3"/>
       <c r="J42" s="3" t="n">
         <v>16</v>
       </c>
       <c r="K42" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="L42" s="3" t="s">
         <v>213</v>
-      </c>
-      <c r="L42" s="3" t="s">
-        <v>214</v>
       </c>
       <c r="M42" s="3" t="n">
         <v>32.2966465</v>
@@ -3258,10 +3269,10 @@
         <v>34.6599276315789</v>
       </c>
       <c r="O42" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="P42" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="Q42" s="4"/>
     </row>
@@ -3276,29 +3287,29 @@
         <v>42</v>
       </c>
       <c r="D43" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="F43" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G43" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="E43" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="F43" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G43" s="3" t="s">
+      <c r="H43" s="3" t="s">
         <v>222</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>223</v>
       </c>
       <c r="I43" s="3"/>
       <c r="J43" s="3" t="n">
         <v>24</v>
       </c>
       <c r="K43" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="L43" s="3" t="s">
         <v>213</v>
-      </c>
-      <c r="L43" s="3" t="s">
-        <v>214</v>
       </c>
       <c r="M43" s="3" t="n">
         <v>32.6406997192308</v>
@@ -3307,10 +3318,10 @@
         <v>35.0272764423077</v>
       </c>
       <c r="O43" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="P43" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Q43" s="4"/>
     </row>
@@ -3325,29 +3336,29 @@
         <v>43</v>
       </c>
       <c r="D44" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="F44" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G44" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="E44" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="F44" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G44" s="3" t="s">
+      <c r="H44" s="3" t="s">
         <v>226</v>
-      </c>
-      <c r="H44" s="3" t="s">
-        <v>227</v>
       </c>
       <c r="I44" s="3"/>
       <c r="J44" s="3" t="n">
         <v>21</v>
       </c>
       <c r="K44" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="L44" s="3" t="s">
         <v>213</v>
-      </c>
-      <c r="L44" s="3" t="s">
-        <v>214</v>
       </c>
       <c r="M44" s="3" t="n">
         <v>32.0573878642857</v>
@@ -3356,10 +3367,10 @@
         <v>35.3856338214286</v>
       </c>
       <c r="O44" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="P44" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="Q44" s="4" t="n">
         <v>1</v>
@@ -3376,29 +3387,29 @@
         <v>44</v>
       </c>
       <c r="D45" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="F45" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G45" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="E45" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="F45" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G45" s="3" t="s">
+      <c r="H45" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="H45" s="3" t="s">
-        <v>231</v>
       </c>
       <c r="I45" s="3"/>
       <c r="J45" s="3" t="n">
         <v>28</v>
       </c>
       <c r="K45" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="L45" s="3" t="s">
         <v>213</v>
-      </c>
-      <c r="L45" s="3" t="s">
-        <v>214</v>
       </c>
       <c r="M45" s="3" t="n">
         <v>34.1861673694915</v>
@@ -3407,10 +3418,10 @@
         <v>30.4976653186441</v>
       </c>
       <c r="O45" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="P45" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="Q45" s="4"/>
     </row>
@@ -3425,29 +3436,29 @@
         <v>45</v>
       </c>
       <c r="D46" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="F46" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G46" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="E46" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="F46" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G46" s="3" t="s">
+      <c r="H46" s="3" t="s">
         <v>234</v>
-      </c>
-      <c r="H46" s="3" t="s">
-        <v>235</v>
       </c>
       <c r="I46" s="3"/>
       <c r="J46" s="3" t="n">
         <v>16</v>
       </c>
       <c r="K46" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L46" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="M46" s="3" t="n">
         <v>35.780619652381</v>
@@ -3456,10 +3467,10 @@
         <v>24.4271275730159</v>
       </c>
       <c r="O46" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="P46" s="3" t="s">
         <v>237</v>
-      </c>
-      <c r="P46" s="3" t="s">
-        <v>238</v>
       </c>
       <c r="Q46" s="4"/>
     </row>
@@ -3474,29 +3485,29 @@
         <v>46</v>
       </c>
       <c r="D47" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="F47" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G47" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="E47" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="F47" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G47" s="3" t="s">
+      <c r="H47" s="3" t="s">
         <v>240</v>
-      </c>
-      <c r="H47" s="3" t="s">
-        <v>241</v>
       </c>
       <c r="I47" s="3"/>
       <c r="J47" s="3" t="n">
         <v>16</v>
       </c>
       <c r="K47" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L47" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="M47" s="3" t="n">
         <v>33.6480191111111</v>
@@ -3505,10 +3516,10 @@
         <v>31.5965783888889</v>
       </c>
       <c r="O47" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="P47" s="3" t="s">
         <v>242</v>
-      </c>
-      <c r="P47" s="3" t="s">
-        <v>243</v>
       </c>
       <c r="Q47" s="4" t="n">
         <v>1</v>
@@ -3525,29 +3536,29 @@
         <v>47</v>
       </c>
       <c r="D48" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="F48" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G48" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="E48" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="F48" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G48" s="3" t="s">
+      <c r="H48" s="3" t="s">
         <v>245</v>
-      </c>
-      <c r="H48" s="3" t="s">
-        <v>246</v>
       </c>
       <c r="I48" s="3"/>
       <c r="J48" s="3" t="n">
         <v>13</v>
       </c>
       <c r="K48" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L48" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="M48" s="3" t="n">
         <v>35.8952308111111</v>
@@ -3556,10 +3567,10 @@
         <v>29.4401928555556</v>
       </c>
       <c r="O48" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="P48" s="3" t="s">
         <v>247</v>
-      </c>
-      <c r="P48" s="3" t="s">
-        <v>248</v>
       </c>
       <c r="Q48" s="4" t="n">
         <v>1</v>
@@ -3576,29 +3587,29 @@
         <v>48</v>
       </c>
       <c r="D49" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="F49" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G49" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="E49" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="F49" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G49" s="3" t="s">
+      <c r="H49" s="3" t="s">
         <v>250</v>
-      </c>
-      <c r="H49" s="3" t="s">
-        <v>251</v>
       </c>
       <c r="I49" s="3"/>
       <c r="J49" s="3" t="n">
         <v>6</v>
       </c>
       <c r="K49" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L49" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="M49" s="3" t="n">
         <v>31.0277102</v>
@@ -3607,10 +3618,10 @@
         <v>37.2690598</v>
       </c>
       <c r="O49" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="P49" s="3" t="s">
         <v>252</v>
-      </c>
-      <c r="P49" s="3" t="s">
-        <v>253</v>
       </c>
       <c r="Q49" s="4"/>
     </row>
@@ -3625,29 +3636,29 @@
         <v>49</v>
       </c>
       <c r="D50" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="F50" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G50" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="E50" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="F50" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G50" s="3" t="s">
+      <c r="H50" s="3" t="s">
         <v>255</v>
-      </c>
-      <c r="H50" s="3" t="s">
-        <v>256</v>
       </c>
       <c r="I50" s="3"/>
       <c r="J50" s="3" t="n">
         <v>6</v>
       </c>
       <c r="K50" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L50" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="M50" s="3" t="n">
         <v>34.9773208333333</v>
@@ -3656,10 +3667,10 @@
         <v>25.5316944</v>
       </c>
       <c r="O50" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="P50" s="3" t="s">
         <v>257</v>
-      </c>
-      <c r="P50" s="3" t="s">
-        <v>258</v>
       </c>
       <c r="Q50" s="4"/>
     </row>
@@ -3674,29 +3685,29 @@
         <v>50</v>
       </c>
       <c r="D51" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="F51" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G51" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="E51" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="F51" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G51" s="3" t="s">
+      <c r="H51" s="3" t="s">
         <v>260</v>
-      </c>
-      <c r="H51" s="3" t="s">
-        <v>261</v>
       </c>
       <c r="I51" s="3"/>
       <c r="J51" s="3" t="n">
         <v>4</v>
       </c>
       <c r="K51" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L51" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="M51" s="3" t="n">
         <v>37.7649163</v>
@@ -3705,10 +3716,10 @@
         <v>26.5137687</v>
       </c>
       <c r="O51" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="P51" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="P51" s="3" t="s">
-        <v>263</v>
       </c>
       <c r="Q51" s="4"/>
     </row>
@@ -3723,29 +3734,29 @@
         <v>51</v>
       </c>
       <c r="D52" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="F52" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G52" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="E52" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="F52" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G52" s="3" t="s">
+      <c r="H52" s="3" t="s">
         <v>265</v>
-      </c>
-      <c r="H52" s="3" t="s">
-        <v>266</v>
       </c>
       <c r="I52" s="3"/>
       <c r="J52" s="3" t="n">
         <v>4</v>
       </c>
       <c r="K52" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L52" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="M52" s="3" t="n">
         <v>35.5407103</v>
@@ -3754,10 +3765,10 @@
         <v>35.7952667</v>
       </c>
       <c r="O52" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="P52" s="3" t="s">
         <v>267</v>
-      </c>
-      <c r="P52" s="3" t="s">
-        <v>268</v>
       </c>
       <c r="Q52" s="4"/>
     </row>
@@ -3772,29 +3783,29 @@
         <v>52</v>
       </c>
       <c r="D53" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="F53" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G53" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="E53" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="F53" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G53" s="3" t="s">
+      <c r="H53" s="3" t="s">
         <v>270</v>
-      </c>
-      <c r="H53" s="3" t="s">
-        <v>271</v>
       </c>
       <c r="I53" s="3"/>
       <c r="J53" s="3" t="n">
         <v>5</v>
       </c>
       <c r="K53" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L53" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="M53" s="3" t="n">
         <v>38.033930725</v>
@@ -3803,10 +3814,10 @@
         <v>25.905193075</v>
       </c>
       <c r="O53" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="P53" s="3" t="s">
         <v>272</v>
-      </c>
-      <c r="P53" s="3" t="s">
-        <v>273</v>
       </c>
       <c r="Q53" s="4"/>
     </row>
@@ -3821,35 +3832,35 @@
         <v>53</v>
       </c>
       <c r="D54" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="F54" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G54" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="E54" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="F54" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G54" s="3" t="s">
+      <c r="H54" s="3" t="s">
         <v>275</v>
-      </c>
-      <c r="H54" s="3" t="s">
-        <v>276</v>
       </c>
       <c r="I54" s="3"/>
       <c r="J54" s="3" t="n">
         <v>3</v>
       </c>
       <c r="K54" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L54" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="O54" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="P54" s="3" t="s">
         <v>277</v>
-      </c>
-      <c r="P54" s="3" t="s">
-        <v>278</v>
       </c>
       <c r="Q54" s="4"/>
     </row>
@@ -3864,29 +3875,29 @@
         <v>54</v>
       </c>
       <c r="D55" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="F55" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G55" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="E55" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="F55" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G55" s="3" t="s">
+      <c r="H55" s="3" t="s">
         <v>280</v>
-      </c>
-      <c r="H55" s="3" t="s">
-        <v>281</v>
       </c>
       <c r="I55" s="3"/>
       <c r="J55" s="3" t="n">
         <v>6</v>
       </c>
       <c r="K55" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L55" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="M55" s="3" t="n">
         <v>39.77852525</v>
@@ -3895,10 +3906,10 @@
         <v>24.5566651</v>
       </c>
       <c r="O55" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="P55" s="3" t="s">
         <v>282</v>
-      </c>
-      <c r="P55" s="3" t="s">
-        <v>283</v>
       </c>
       <c r="Q55" s="4"/>
     </row>
@@ -3913,29 +3924,29 @@
         <v>55</v>
       </c>
       <c r="D56" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="F56" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G56" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="E56" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="F56" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G56" s="3" t="s">
+      <c r="H56" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="H56" s="3" t="s">
-        <v>286</v>
       </c>
       <c r="I56" s="3"/>
       <c r="J56" s="3" t="n">
         <v>4</v>
       </c>
       <c r="K56" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L56" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="M56" s="3" t="n">
         <v>38.8302656777778</v>
@@ -3944,10 +3955,10 @@
         <v>27.4323937222222</v>
       </c>
       <c r="O56" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="P56" s="3" t="s">
         <v>287</v>
-      </c>
-      <c r="P56" s="3" t="s">
-        <v>288</v>
       </c>
       <c r="Q56" s="4"/>
     </row>
@@ -3962,29 +3973,29 @@
         <v>56</v>
       </c>
       <c r="D57" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="F57" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G57" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="E57" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="F57" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G57" s="3" t="s">
+      <c r="H57" s="3" t="s">
         <v>290</v>
-      </c>
-      <c r="H57" s="3" t="s">
-        <v>291</v>
       </c>
       <c r="I57" s="3"/>
       <c r="J57" s="3" t="n">
         <v>3</v>
       </c>
       <c r="K57" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L57" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="M57" s="3" t="n">
         <v>35.240117</v>
@@ -3993,10 +4004,10 @@
         <v>24.8092691</v>
       </c>
       <c r="O57" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="P57" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="Q57" s="4"/>
     </row>
@@ -4011,35 +4022,35 @@
         <v>57</v>
       </c>
       <c r="D58" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="F58" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G58" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="E58" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="F58" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G58" s="3" t="s">
+      <c r="H58" s="3" t="s">
         <v>294</v>
-      </c>
-      <c r="H58" s="3" t="s">
-        <v>295</v>
       </c>
       <c r="I58" s="3"/>
       <c r="J58" s="3" t="n">
         <v>1</v>
       </c>
       <c r="K58" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L58" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="O58" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="P58" s="3" t="s">
         <v>296</v>
-      </c>
-      <c r="P58" s="3" t="s">
-        <v>297</v>
       </c>
       <c r="Q58" s="4"/>
     </row>
@@ -4054,29 +4065,29 @@
         <v>58</v>
       </c>
       <c r="D59" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="F59" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G59" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="E59" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="F59" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G59" s="3" t="s">
+      <c r="H59" s="3" t="s">
         <v>299</v>
-      </c>
-      <c r="H59" s="3" t="s">
-        <v>300</v>
       </c>
       <c r="I59" s="3"/>
       <c r="J59" s="3" t="n">
         <v>13</v>
       </c>
       <c r="K59" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L59" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="M59" s="3" t="n">
         <v>30.6318454833334</v>
@@ -4085,10 +4096,10 @@
         <v>32.0784964763889</v>
       </c>
       <c r="O59" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="P59" s="3" t="s">
         <v>301</v>
-      </c>
-      <c r="P59" s="3" t="s">
-        <v>302</v>
       </c>
       <c r="Q59" s="4"/>
     </row>
@@ -4103,35 +4114,35 @@
         <v>59</v>
       </c>
       <c r="D60" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="F60" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G60" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="E60" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="F60" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G60" s="3" t="s">
+      <c r="H60" s="3" t="s">
         <v>304</v>
-      </c>
-      <c r="H60" s="3" t="s">
-        <v>305</v>
       </c>
       <c r="I60" s="3"/>
       <c r="J60" s="3" t="n">
         <v>5</v>
       </c>
       <c r="K60" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L60" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="O60" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="P60" s="3" t="s">
         <v>306</v>
-      </c>
-      <c r="P60" s="3" t="s">
-        <v>307</v>
       </c>
       <c r="Q60" s="4"/>
     </row>
@@ -4146,29 +4157,29 @@
         <v>60</v>
       </c>
       <c r="D61" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="F61" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G61" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="E61" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="F61" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G61" s="3" t="s">
+      <c r="H61" s="3" t="s">
         <v>309</v>
-      </c>
-      <c r="H61" s="3" t="s">
-        <v>310</v>
       </c>
       <c r="I61" s="3"/>
       <c r="J61" s="3" t="n">
         <v>5</v>
       </c>
       <c r="K61" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L61" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="M61" s="3" t="n">
         <v>34.622887888889</v>
@@ -4177,10 +4188,10 @@
         <v>37.9289433703703</v>
       </c>
       <c r="O61" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="P61" s="3" t="s">
         <v>311</v>
-      </c>
-      <c r="P61" s="3" t="s">
-        <v>312</v>
       </c>
       <c r="Q61" s="4"/>
     </row>
@@ -4195,29 +4206,29 @@
         <v>61</v>
       </c>
       <c r="D62" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="F62" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G62" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="E62" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="F62" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G62" s="3" t="s">
+      <c r="H62" s="3" t="s">
         <v>314</v>
-      </c>
-      <c r="H62" s="3" t="s">
-        <v>315</v>
       </c>
       <c r="I62" s="3"/>
       <c r="J62" s="3" t="n">
         <v>3</v>
       </c>
       <c r="K62" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L62" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="M62" s="3" t="n">
         <v>31.771666666667</v>
@@ -4226,10 +4237,10 @@
         <v>35.228611111111</v>
       </c>
       <c r="O62" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="P62" s="3" t="s">
         <v>316</v>
-      </c>
-      <c r="P62" s="3" t="s">
-        <v>317</v>
       </c>
       <c r="Q62" s="4"/>
     </row>
@@ -4244,35 +4255,35 @@
         <v>62</v>
       </c>
       <c r="D63" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="F63" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G63" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="E63" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="F63" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G63" s="3" t="s">
+      <c r="H63" s="3" t="s">
         <v>319</v>
-      </c>
-      <c r="H63" s="3" t="s">
-        <v>320</v>
       </c>
       <c r="I63" s="3"/>
       <c r="J63" s="3" t="n">
         <v>5</v>
       </c>
       <c r="K63" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L63" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="O63" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="P63" s="3" t="s">
         <v>321</v>
-      </c>
-      <c r="P63" s="3" t="s">
-        <v>322</v>
       </c>
       <c r="Q63" s="4"/>
     </row>
@@ -4287,35 +4298,35 @@
         <v>63</v>
       </c>
       <c r="D64" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="F64" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G64" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="E64" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="F64" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G64" s="3" t="s">
+      <c r="H64" s="3" t="s">
         <v>324</v>
-      </c>
-      <c r="H64" s="3" t="s">
-        <v>325</v>
       </c>
       <c r="I64" s="3"/>
       <c r="J64" s="3" t="n">
         <v>1</v>
       </c>
       <c r="K64" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L64" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="O64" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="P64" s="3" t="s">
         <v>326</v>
-      </c>
-      <c r="P64" s="3" t="s">
-        <v>327</v>
       </c>
       <c r="Q64" s="4"/>
     </row>
@@ -4330,35 +4341,35 @@
         <v>64</v>
       </c>
       <c r="D65" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="F65" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G65" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="E65" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="F65" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G65" s="3" t="s">
+      <c r="H65" s="3" t="s">
         <v>329</v>
-      </c>
-      <c r="H65" s="3" t="s">
-        <v>330</v>
       </c>
       <c r="I65" s="3"/>
       <c r="J65" s="3" t="n">
         <v>1</v>
       </c>
       <c r="K65" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L65" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="O65" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="P65" s="3" t="s">
         <v>331</v>
-      </c>
-      <c r="P65" s="3" t="s">
-        <v>332</v>
       </c>
       <c r="Q65" s="4"/>
     </row>
@@ -4373,29 +4384,29 @@
         <v>65</v>
       </c>
       <c r="D66" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="F66" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G66" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="E66" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="F66" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G66" s="3" t="s">
+      <c r="H66" s="3" t="s">
         <v>334</v>
-      </c>
-      <c r="H66" s="3" t="s">
-        <v>335</v>
       </c>
       <c r="I66" s="3"/>
       <c r="J66" s="3" t="n">
         <v>1</v>
       </c>
       <c r="K66" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L66" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="M66" s="3" t="n">
         <v>26.820553</v>
@@ -4404,10 +4415,10 @@
         <v>30.802498</v>
       </c>
       <c r="O66" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="P66" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Q66" s="4"/>
     </row>
@@ -4422,29 +4433,29 @@
         <v>66</v>
       </c>
       <c r="D67" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="F67" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G67" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="E67" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="F67" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G67" s="3" t="s">
+      <c r="H67" s="3" t="s">
         <v>338</v>
-      </c>
-      <c r="H67" s="3" t="s">
-        <v>339</v>
       </c>
       <c r="I67" s="3"/>
       <c r="J67" s="3" t="n">
         <v>22</v>
       </c>
       <c r="K67" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="L67" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="L67" s="3" t="s">
-        <v>129</v>
       </c>
       <c r="M67" s="3" t="n">
         <v>34.7078413805556</v>
@@ -4453,10 +4464,10 @@
         <v>33.5147325425926</v>
       </c>
       <c r="O67" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="P67" s="3" t="s">
         <v>340</v>
-      </c>
-      <c r="P67" s="3" t="s">
-        <v>341</v>
       </c>
       <c r="Q67" s="4" t="n">
         <v>1</v>
@@ -4475,7 +4486,7 @@
       <c r="A71" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:P67"/>
+  <autoFilter ref="B1:Q67"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
added columns to books file
</commit_message>
<xml_diff>
--- a/documentation/books.xlsx
+++ b/documentation/books.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$Q$67</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$P$67</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$P$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$Q$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$B$1:$O$67</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="346">
   <si>
     <t xml:space="preserve">bible</t>
   </si>
@@ -70,6 +70,21 @@
   </si>
   <si>
     <t xml:space="preserve">sexual_annotation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">part</t>
+  </si>
+  <si>
+    <t xml:space="preserve">author</t>
+  </si>
+  <si>
+    <t xml:space="preserve">language</t>
+  </si>
+  <si>
+    <t xml:space="preserve">period_produced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">period_setting</t>
   </si>
   <si>
     <t xml:space="preserve">Génesis</t>
@@ -1187,13 +1202,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q71"/>
+  <dimension ref="A1:V71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q10" activeCellId="0" sqref="Q10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O10" activeCellId="0" sqref="O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.8"/>
+  </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
@@ -1242,6 +1260,21 @@
       <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="R1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
@@ -1254,29 +1287,29 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F2" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3" t="n">
         <v>50</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="M2" s="3" t="n">
         <v>32.6156867451613</v>
@@ -1285,14 +1318,15 @@
         <v>36.7930834290323</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="Q2" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="R2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
@@ -1305,29 +1339,29 @@
         <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F3" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3" t="n">
         <v>40</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="M3" s="3" t="n">
         <v>30.4699688976191</v>
@@ -1336,12 +1370,13 @@
         <v>33.8432804079365</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
@@ -1354,29 +1389,29 @@
         <v>3</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F4" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3" t="n">
         <v>27</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="M4" s="3" t="n">
         <v>30.5217654</v>
@@ -1385,12 +1420,13 @@
         <v>34.112561</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
@@ -1403,29 +1439,29 @@
         <v>4</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F5" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3" t="n">
         <v>36</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="M5" s="3" t="n">
         <v>31.2216179928572</v>
@@ -1434,12 +1470,13 @@
         <v>34.8414332857143</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
@@ -1452,29 +1489,29 @@
         <v>5</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F6" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3" t="n">
         <v>34</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="M6" s="3" t="n">
         <v>31.5061064931373</v>
@@ -1483,12 +1520,13 @@
         <v>35.735247453268</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
@@ -1501,29 +1539,29 @@
         <v>6</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F7" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3" t="n">
         <v>24</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="M7" s="3" t="n">
         <v>31.7040713934426</v>
@@ -1532,12 +1570,13 @@
         <v>34.9903732852459</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
@@ -1550,29 +1589,29 @@
         <v>7</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F8" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3" t="n">
         <v>21</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="M8" s="3" t="n">
         <v>31.7295635169811</v>
@@ -1581,12 +1620,13 @@
         <v>35.467874809434</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
@@ -1599,29 +1639,29 @@
         <v>8</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F9" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3" t="n">
         <v>4</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="M9" s="3" t="n">
         <v>29.8573287</v>
@@ -1630,14 +1670,15 @@
         <v>33.6188508333333</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="Q9" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="R9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
@@ -1650,29 +1691,29 @@
         <v>9</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F10" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3" t="n">
         <v>31</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="M10" s="3" t="n">
         <v>31.5980145176471</v>
@@ -1681,12 +1722,13 @@
         <v>35.0461610117647</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
@@ -1699,29 +1741,29 @@
         <v>10</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F11" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3" t="n">
         <v>24</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="M11" s="3" t="n">
         <v>32.2183292375</v>
@@ -1730,12 +1772,13 @@
         <v>35.26103851875</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
@@ -1748,29 +1791,29 @@
         <v>11</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F12" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3" t="n">
         <v>22</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="M12" s="3" t="n">
         <v>31.8670741222222</v>
@@ -1779,12 +1822,13 @@
         <v>35.1852309356481</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
@@ -1797,29 +1841,29 @@
         <v>12</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F13" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3" t="n">
         <v>25</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="M13" s="3" t="n">
         <v>31.9348416753968</v>
@@ -1828,12 +1872,13 @@
         <v>36.3334837740741</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
@@ -1846,29 +1891,29 @@
         <v>13</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F14" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="I14" s="3"/>
       <c r="J14" s="3" t="n">
         <v>29</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="M14" s="3" t="n">
         <v>32.0105521231884</v>
@@ -1877,12 +1922,13 @@
         <v>36.031745213285</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
@@ -1895,29 +1941,29 @@
         <v>14</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F15" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I15" s="3"/>
       <c r="J15" s="3" t="n">
         <v>36</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="M15" s="3" t="n">
         <v>32.0012473111111</v>
@@ -1926,12 +1972,13 @@
         <v>35.8507288237473</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="P15" s="3" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
@@ -1944,29 +1991,29 @@
         <v>15</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F16" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="I16" s="3"/>
       <c r="J16" s="3" t="n">
         <v>10</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="M16" s="3" t="n">
         <v>32.320034525</v>
@@ -1975,12 +2022,13 @@
         <v>37.691306715</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="Q16" s="4"/>
+      <c r="R16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
@@ -1993,29 +2041,29 @@
         <v>16</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F17" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="I17" s="3"/>
       <c r="J17" s="3" t="n">
         <v>13</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="M17" s="3" t="n">
         <v>31.3170995516129</v>
@@ -2024,12 +2072,13 @@
         <v>37.0320123806452</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
@@ -2042,29 +2091,29 @@
         <v>17</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F18" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="I18" s="3"/>
       <c r="J18" s="3" t="n">
         <v>10</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="M18" s="3" t="n">
         <v>29.276842025</v>
@@ -2073,12 +2122,13 @@
         <v>40.9689593</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="P18" s="3" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
@@ -2091,29 +2141,29 @@
         <v>18</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F19" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="I19" s="3"/>
       <c r="J19" s="3" t="n">
         <v>42</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="M19" s="3" t="n">
         <v>19.865082</v>
@@ -2122,14 +2172,15 @@
         <v>38.3640435</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="Q19" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="R19" s="4"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="n">
@@ -2142,29 +2193,29 @@
         <v>19</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F20" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="I20" s="3"/>
       <c r="J20" s="3" t="n">
         <v>150</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="M20" s="3" t="n">
         <v>30.9532842802083</v>
@@ -2173,14 +2224,15 @@
         <v>35.4313175003472</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="P20" s="3" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="Q20" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="R20" s="4"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="n">
@@ -2193,29 +2245,29 @@
         <v>20</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F21" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="I21" s="3"/>
       <c r="J21" s="3" t="n">
         <v>31</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="M21" s="3" t="n">
         <v>29.9232731333333</v>
@@ -2224,12 +2276,13 @@
         <v>33.6192164666667</v>
       </c>
       <c r="O21" s="3" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="P21" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="Q21" s="4"/>
+      <c r="R21" s="4"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="n">
@@ -2242,29 +2295,29 @@
         <v>21</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F22" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="I22" s="3"/>
       <c r="J22" s="3" t="n">
         <v>12</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="M22" s="3" t="n">
         <v>32.0003456666667</v>
@@ -2273,12 +2326,13 @@
         <v>35.228163</v>
       </c>
       <c r="O22" s="3" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="P22" s="3" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="Q22" s="4"/>
+      <c r="R22" s="4"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="n">
@@ -2291,29 +2345,29 @@
         <v>22</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F23" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="I23" s="3"/>
       <c r="J23" s="3" t="n">
         <v>8</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="M23" s="3" t="n">
         <v>32.2361352458334</v>
@@ -2322,14 +2376,15 @@
         <v>35.5485861263889</v>
       </c>
       <c r="O23" s="3" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="P23" s="3" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="Q23" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="R23" s="4"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="n">
@@ -2342,29 +2397,29 @@
         <v>23</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F24" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="I24" s="3"/>
       <c r="J24" s="3" t="n">
         <v>66</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="M24" s="3" t="n">
         <v>31.558286685034</v>
@@ -2373,12 +2428,13 @@
         <v>36.2484380798186</v>
       </c>
       <c r="O24" s="3" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="P24" s="3" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="Q24" s="4"/>
+      <c r="R24" s="4"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="n">
@@ -2391,29 +2447,29 @@
         <v>24</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F25" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="I25" s="3"/>
       <c r="J25" s="3" t="n">
         <v>52</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="M25" s="3" t="n">
         <v>32.340919558642</v>
@@ -2422,12 +2478,13 @@
         <v>35.4158287465021</v>
       </c>
       <c r="O25" s="3" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="P25" s="3" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="Q25" s="4"/>
+      <c r="R25" s="4"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="n">
@@ -2440,29 +2497,29 @@
         <v>25</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F26" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="I26" s="3"/>
       <c r="J26" s="3" t="n">
         <v>5</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="M26" s="3" t="n">
         <v>31.7260940111112</v>
@@ -2471,12 +2528,13 @@
         <v>35.2035639185185</v>
       </c>
       <c r="O26" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="P26" s="3" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="Q26" s="4"/>
+      <c r="R26" s="4"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="n">
@@ -2489,29 +2547,29 @@
         <v>26</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F27" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="I27" s="3"/>
       <c r="J27" s="3" t="n">
         <v>48</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="M27" s="3" t="n">
         <v>31.5987830993464</v>
@@ -2520,14 +2578,15 @@
         <v>35.4612548551198</v>
       </c>
       <c r="O27" s="3" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="P27" s="3" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="Q27" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="R27" s="4"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="n">
@@ -2540,29 +2599,29 @@
         <v>27</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F28" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="I28" s="3"/>
       <c r="J28" s="3" t="n">
         <v>12</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="M28" s="3" t="n">
         <v>30.0115475244445</v>
@@ -2571,12 +2630,13 @@
         <v>36.9681489007407</v>
       </c>
       <c r="O28" s="3" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="P28" s="3" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="n">
@@ -2589,29 +2649,29 @@
         <v>28</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F29" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="I29" s="3"/>
       <c r="J29" s="3" t="n">
         <v>14</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="M29" s="3" t="n">
         <v>31.9816348666667</v>
@@ -2620,12 +2680,13 @@
         <v>35.2501034333333</v>
       </c>
       <c r="O29" s="3" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="P29" s="3" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="n">
@@ -2638,29 +2699,29 @@
         <v>29</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F30" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="I30" s="3"/>
       <c r="J30" s="3" t="n">
         <v>3</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="M30" s="3" t="n">
         <v>31.8152915888889</v>
@@ -2669,12 +2730,13 @@
         <v>33.3907050509259</v>
       </c>
       <c r="O30" s="3" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="P30" s="3" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="Q30" s="4"/>
+      <c r="R30" s="4"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="n">
@@ -2687,29 +2749,29 @@
         <v>30</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F31" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="I31" s="3"/>
       <c r="J31" s="3" t="n">
         <v>9</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="M31" s="3" t="n">
         <v>31.8051863706667</v>
@@ -2718,12 +2780,13 @@
         <v>35.0574446284444</v>
       </c>
       <c r="O31" s="3" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="P31" s="3" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="Q31" s="4"/>
+      <c r="R31" s="4"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="n">
@@ -2736,29 +2799,29 @@
         <v>31</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F32" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="I32" s="3"/>
       <c r="J32" s="3" t="n">
         <v>1</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="M32" s="3" t="n">
         <v>31.6259671166667</v>
@@ -2767,12 +2830,13 @@
         <v>35.2103703711111</v>
       </c>
       <c r="O32" s="3" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="P32" s="3" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="Q32" s="4"/>
+      <c r="R32" s="4"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="n">
@@ -2785,29 +2849,29 @@
         <v>32</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F33" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="I33" s="3"/>
       <c r="J33" s="3" t="n">
         <v>4</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="M33" s="3" t="n">
         <v>36.6525328333333</v>
@@ -2816,12 +2880,13 @@
         <v>34.9298637666667</v>
       </c>
       <c r="O33" s="3" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="P33" s="3" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="Q33" s="4"/>
+      <c r="R33" s="4"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="n">
@@ -2834,29 +2899,29 @@
         <v>33</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F34" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="I34" s="3"/>
       <c r="J34" s="3" t="n">
         <v>7</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="M34" s="3" t="n">
         <v>32.0123840119048</v>
@@ -2865,12 +2930,13 @@
         <v>36.2378762579365</v>
       </c>
       <c r="O34" s="3" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="P34" s="3" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="Q34" s="4"/>
+      <c r="R34" s="4"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="n">
@@ -2883,29 +2949,29 @@
         <v>34</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F35" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="I35" s="3"/>
       <c r="J35" s="3" t="n">
         <v>3</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="L35" s="3" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="M35" s="3" t="n">
         <v>30.02499748</v>
@@ -2914,14 +2980,15 @@
         <v>33.51317685</v>
       </c>
       <c r="O35" s="3" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="P35" s="3" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="Q35" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="R35" s="4"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="n">
@@ -2934,29 +3001,29 @@
         <v>35</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F36" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="I36" s="3"/>
       <c r="J36" s="3" t="n">
         <v>3</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="L36" s="3" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="M36" s="3" t="n">
         <v>31.8736</v>
@@ -2965,14 +3032,15 @@
         <v>35.749305</v>
       </c>
       <c r="O36" s="3" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="P36" s="3" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="Q36" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="R36" s="4"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="n">
@@ -2985,29 +3053,29 @@
         <v>36</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F37" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="I37" s="3"/>
       <c r="J37" s="3" t="n">
         <v>3</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="L37" s="3" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="M37" s="3" t="n">
         <v>30.7004767060606</v>
@@ -3016,14 +3084,15 @@
         <v>35.3679248191919</v>
       </c>
       <c r="O37" s="3" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="P37" s="3" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="Q37" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="R37" s="4"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="n">
@@ -3036,29 +3105,29 @@
         <v>37</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F38" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="I38" s="3"/>
       <c r="J38" s="3" t="n">
         <v>2</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="L38" s="3" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="M38" s="3" t="n">
         <v>30.7391216</v>
@@ -3067,14 +3136,15 @@
         <v>34.1192041</v>
       </c>
       <c r="O38" s="3" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="P38" s="3" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="Q38" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="R38" s="4"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="n">
@@ -3087,29 +3157,29 @@
         <v>38</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F39" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="I39" s="3"/>
       <c r="J39" s="3" t="n">
         <v>14</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="L39" s="3" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="M39" s="3" t="n">
         <v>32.4563420913581</v>
@@ -3118,14 +3188,15 @@
         <v>34.6885989967078</v>
       </c>
       <c r="O39" s="3" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="P39" s="3" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="Q39" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="R39" s="4"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="n">
@@ -3138,29 +3209,29 @@
         <v>39</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F40" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="I40" s="3"/>
       <c r="J40" s="3" t="n">
         <v>4</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="L40" s="3" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="M40" s="3" t="n">
         <v>31.2363364</v>
@@ -3169,12 +3240,13 @@
         <v>34.9578466</v>
       </c>
       <c r="O40" s="3" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="P40" s="3" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="Q40" s="4"/>
+      <c r="R40" s="4"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="n">
@@ -3187,29 +3259,29 @@
         <v>40</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="F41" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="I41" s="3"/>
       <c r="J41" s="3" t="n">
         <v>28</v>
       </c>
       <c r="K41" s="3" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="L41" s="3" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="M41" s="3" t="n">
         <v>32.3601598061729</v>
@@ -3218,14 +3290,15 @@
         <v>35.0756762263374</v>
       </c>
       <c r="O41" s="3" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="P41" s="3" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="Q41" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="R41" s="4"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="n">
@@ -3238,29 +3311,29 @@
         <v>41</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="F42" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="I42" s="3"/>
       <c r="J42" s="3" t="n">
         <v>16</v>
       </c>
       <c r="K42" s="3" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="L42" s="3" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="M42" s="3" t="n">
         <v>32.2966465</v>
@@ -3269,12 +3342,13 @@
         <v>34.6599276315789</v>
       </c>
       <c r="O42" s="3" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="P42" s="3" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="Q42" s="4"/>
+      <c r="R42" s="4"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="n">
@@ -3287,29 +3361,29 @@
         <v>42</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="F43" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="I43" s="3"/>
       <c r="J43" s="3" t="n">
         <v>24</v>
       </c>
       <c r="K43" s="3" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="L43" s="3" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="M43" s="3" t="n">
         <v>32.6406997192308</v>
@@ -3318,12 +3392,13 @@
         <v>35.0272764423077</v>
       </c>
       <c r="O43" s="3" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="P43" s="3" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="Q43" s="4"/>
+      <c r="R43" s="4"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="n">
@@ -3336,29 +3411,29 @@
         <v>43</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="F44" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="I44" s="3"/>
       <c r="J44" s="3" t="n">
         <v>21</v>
       </c>
       <c r="K44" s="3" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="L44" s="3" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="M44" s="3" t="n">
         <v>32.0573878642857</v>
@@ -3367,14 +3442,15 @@
         <v>35.3856338214286</v>
       </c>
       <c r="O44" s="3" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="P44" s="3" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="Q44" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="R44" s="4"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="n">
@@ -3387,29 +3463,29 @@
         <v>44</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="F45" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="I45" s="3"/>
       <c r="J45" s="3" t="n">
         <v>28</v>
       </c>
       <c r="K45" s="3" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="L45" s="3" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="M45" s="3" t="n">
         <v>34.1861673694915</v>
@@ -3418,12 +3494,13 @@
         <v>30.4976653186441</v>
       </c>
       <c r="O45" s="3" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="P45" s="3" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="Q45" s="4"/>
+      <c r="R45" s="4"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="n">
@@ -3436,29 +3513,29 @@
         <v>45</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="F46" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="I46" s="3"/>
       <c r="J46" s="3" t="n">
         <v>16</v>
       </c>
       <c r="K46" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="L46" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="M46" s="3" t="n">
         <v>35.780619652381</v>
@@ -3467,12 +3544,13 @@
         <v>24.4271275730159</v>
       </c>
       <c r="O46" s="3" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="P46" s="3" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="Q46" s="4"/>
+      <c r="R46" s="4"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="n">
@@ -3485,29 +3563,29 @@
         <v>46</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="F47" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="I47" s="3"/>
       <c r="J47" s="3" t="n">
         <v>16</v>
       </c>
       <c r="K47" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="L47" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="M47" s="3" t="n">
         <v>33.6480191111111</v>
@@ -3516,14 +3594,15 @@
         <v>31.5965783888889</v>
       </c>
       <c r="O47" s="3" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="P47" s="3" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="Q47" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="R47" s="4"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="n">
@@ -3536,29 +3615,29 @@
         <v>47</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="F48" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="I48" s="3"/>
       <c r="J48" s="3" t="n">
         <v>13</v>
       </c>
       <c r="K48" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="L48" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="M48" s="3" t="n">
         <v>35.8952308111111</v>
@@ -3567,14 +3646,15 @@
         <v>29.4401928555556</v>
       </c>
       <c r="O48" s="3" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="P48" s="3" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="Q48" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="R48" s="4"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="n">
@@ -3587,29 +3667,29 @@
         <v>48</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="F49" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="I49" s="3"/>
       <c r="J49" s="3" t="n">
         <v>6</v>
       </c>
       <c r="K49" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="L49" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="M49" s="3" t="n">
         <v>31.0277102</v>
@@ -3618,12 +3698,13 @@
         <v>37.2690598</v>
       </c>
       <c r="O49" s="3" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="P49" s="3" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="Q49" s="4"/>
+      <c r="R49" s="4"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="n">
@@ -3636,29 +3717,29 @@
         <v>49</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="F50" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="I50" s="3"/>
       <c r="J50" s="3" t="n">
         <v>6</v>
       </c>
       <c r="K50" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="L50" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="M50" s="3" t="n">
         <v>34.9773208333333</v>
@@ -3667,12 +3748,13 @@
         <v>25.5316944</v>
       </c>
       <c r="O50" s="3" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="P50" s="3" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="Q50" s="4"/>
+      <c r="R50" s="4"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="n">
@@ -3685,29 +3767,29 @@
         <v>50</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="F51" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="I51" s="3"/>
       <c r="J51" s="3" t="n">
         <v>4</v>
       </c>
       <c r="K51" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="L51" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="M51" s="3" t="n">
         <v>37.7649163</v>
@@ -3716,12 +3798,13 @@
         <v>26.5137687</v>
       </c>
       <c r="O51" s="3" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="P51" s="3" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="Q51" s="4"/>
+      <c r="R51" s="4"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="n">
@@ -3734,29 +3817,29 @@
         <v>51</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="F52" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="I52" s="3"/>
       <c r="J52" s="3" t="n">
         <v>4</v>
       </c>
       <c r="K52" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="L52" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="M52" s="3" t="n">
         <v>35.5407103</v>
@@ -3765,12 +3848,13 @@
         <v>35.7952667</v>
       </c>
       <c r="O52" s="3" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="P52" s="3" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="Q52" s="4"/>
+      <c r="R52" s="4"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="n">
@@ -3783,29 +3867,29 @@
         <v>52</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="F53" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="I53" s="3"/>
       <c r="J53" s="3" t="n">
         <v>5</v>
       </c>
       <c r="K53" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="L53" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="M53" s="3" t="n">
         <v>38.033930725</v>
@@ -3814,12 +3898,13 @@
         <v>25.905193075</v>
       </c>
       <c r="O53" s="3" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="P53" s="3" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="Q53" s="4"/>
+      <c r="R53" s="4"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="n">
@@ -3832,37 +3917,38 @@
         <v>53</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="F54" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="I54" s="3"/>
       <c r="J54" s="3" t="n">
         <v>3</v>
       </c>
       <c r="K54" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="L54" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="O54" s="3" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="P54" s="3" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="Q54" s="4"/>
+      <c r="R54" s="4"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="n">
@@ -3875,29 +3961,29 @@
         <v>54</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="F55" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="I55" s="3"/>
       <c r="J55" s="3" t="n">
         <v>6</v>
       </c>
       <c r="K55" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="L55" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="M55" s="3" t="n">
         <v>39.77852525</v>
@@ -3906,12 +3992,13 @@
         <v>24.5566651</v>
       </c>
       <c r="O55" s="3" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="P55" s="3" t="s">
-        <v>282</v>
+        <v>287</v>
       </c>
       <c r="Q55" s="4"/>
+      <c r="R55" s="4"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="n">
@@ -3924,29 +4011,29 @@
         <v>55</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="F56" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="I56" s="3"/>
       <c r="J56" s="3" t="n">
         <v>4</v>
       </c>
       <c r="K56" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="L56" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="M56" s="3" t="n">
         <v>38.8302656777778</v>
@@ -3955,12 +4042,13 @@
         <v>27.4323937222222</v>
       </c>
       <c r="O56" s="3" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
       <c r="P56" s="3" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="Q56" s="4"/>
+      <c r="R56" s="4"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="n">
@@ -3973,29 +4061,29 @@
         <v>56</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="F57" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="I57" s="3"/>
       <c r="J57" s="3" t="n">
         <v>3</v>
       </c>
       <c r="K57" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="L57" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="M57" s="3" t="n">
         <v>35.240117</v>
@@ -4004,12 +4092,13 @@
         <v>24.8092691</v>
       </c>
       <c r="O57" s="3" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="P57" s="3" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="Q57" s="4"/>
+      <c r="R57" s="4"/>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="n">
@@ -4022,37 +4111,38 @@
         <v>57</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="F58" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="I58" s="3"/>
       <c r="J58" s="3" t="n">
         <v>1</v>
       </c>
       <c r="K58" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="L58" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="O58" s="3" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="P58" s="3" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="Q58" s="4"/>
+      <c r="R58" s="4"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="n">
@@ -4065,29 +4155,29 @@
         <v>58</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="F59" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="I59" s="3"/>
       <c r="J59" s="3" t="n">
         <v>13</v>
       </c>
       <c r="K59" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="L59" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="M59" s="3" t="n">
         <v>30.6318454833334</v>
@@ -4096,12 +4186,13 @@
         <v>32.0784964763889</v>
       </c>
       <c r="O59" s="3" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="P59" s="3" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="Q59" s="4"/>
+      <c r="R59" s="4"/>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="n">
@@ -4114,37 +4205,38 @@
         <v>59</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="F60" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="I60" s="3"/>
       <c r="J60" s="3" t="n">
         <v>5</v>
       </c>
       <c r="K60" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="L60" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="O60" s="3" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="P60" s="3" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="Q60" s="4"/>
+      <c r="R60" s="4"/>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="n">
@@ -4157,29 +4249,29 @@
         <v>60</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="F61" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="I61" s="3"/>
       <c r="J61" s="3" t="n">
         <v>5</v>
       </c>
       <c r="K61" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="L61" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="M61" s="3" t="n">
         <v>34.622887888889</v>
@@ -4188,12 +4280,13 @@
         <v>37.9289433703703</v>
       </c>
       <c r="O61" s="3" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="P61" s="3" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="Q61" s="4"/>
+      <c r="R61" s="4"/>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="n">
@@ -4206,29 +4299,29 @@
         <v>61</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="F62" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="H62" s="3" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="I62" s="3"/>
       <c r="J62" s="3" t="n">
         <v>3</v>
       </c>
       <c r="K62" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="L62" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="M62" s="3" t="n">
         <v>31.771666666667</v>
@@ -4237,12 +4330,13 @@
         <v>35.228611111111</v>
       </c>
       <c r="O62" s="3" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="P62" s="3" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="Q62" s="4"/>
+      <c r="R62" s="4"/>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="n">
@@ -4255,37 +4349,38 @@
         <v>62</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="F63" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="I63" s="3"/>
       <c r="J63" s="3" t="n">
         <v>5</v>
       </c>
       <c r="K63" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="L63" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="O63" s="3" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="P63" s="3" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="Q63" s="4"/>
+      <c r="R63" s="4"/>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="n">
@@ -4298,37 +4393,38 @@
         <v>63</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="F64" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
       <c r="I64" s="3"/>
       <c r="J64" s="3" t="n">
         <v>1</v>
       </c>
       <c r="K64" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="L64" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="O64" s="3" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="P64" s="3" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="Q64" s="4"/>
+      <c r="R64" s="4"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="n">
@@ -4341,37 +4437,38 @@
         <v>64</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="F65" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="I65" s="3"/>
       <c r="J65" s="3" t="n">
         <v>1</v>
       </c>
       <c r="K65" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="L65" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="O65" s="3" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="P65" s="3" t="s">
-        <v>331</v>
+        <v>336</v>
       </c>
       <c r="Q65" s="4"/>
+      <c r="R65" s="4"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="n">
@@ -4384,29 +4481,29 @@
         <v>65</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="F66" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="I66" s="3"/>
       <c r="J66" s="3" t="n">
         <v>1</v>
       </c>
       <c r="K66" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="L66" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="M66" s="3" t="n">
         <v>26.820553</v>
@@ -4415,12 +4512,13 @@
         <v>30.802498</v>
       </c>
       <c r="O66" s="3" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="P66" s="3" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="Q66" s="4"/>
+      <c r="R66" s="4"/>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="n">
@@ -4433,29 +4531,29 @@
         <v>66</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>336</v>
+        <v>341</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="F67" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>337</v>
+        <v>342</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>338</v>
+        <v>343</v>
       </c>
       <c r="I67" s="3"/>
       <c r="J67" s="3" t="n">
         <v>22</v>
       </c>
       <c r="K67" s="3" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="L67" s="3" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="M67" s="3" t="n">
         <v>34.7078413805556</v>
@@ -4464,14 +4562,15 @@
         <v>33.5147325425926</v>
       </c>
       <c r="O67" s="3" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
       <c r="P67" s="3" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
       <c r="Q67" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="R67" s="4"/>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2"/>
@@ -4486,7 +4585,7 @@
       <c r="A71" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:Q67"/>
+  <autoFilter ref="B1:P67"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
comenzando anotación de la carta de romanos
</commit_message>
<xml_diff>
--- a/documentation/books.xlsx
+++ b/documentation/books.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$Q$67</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$P$67</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$P$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$Q$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$B$1:$O$67</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -1229,14 +1229,14 @@
   <dimension ref="A1:AMJ71"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="I58" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="E58" activeCellId="0" sqref="E58"/>
-      <selection pane="bottomRight" activeCell="J75" activeCellId="0" sqref="J75"/>
+      <selection pane="bottomLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="bottomRight" activeCell="Q12" activeCellId="0" sqref="Q12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="10.77"/>
@@ -1797,7 +1797,9 @@
       <c r="P10" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="Q10" s="4"/>
+      <c r="Q10" s="4" t="n">
+        <v>0.5</v>
+      </c>
       <c r="R10" s="4" t="s">
         <v>55</v>
       </c>
@@ -1852,7 +1854,9 @@
       <c r="P11" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="Q11" s="4"/>
+      <c r="Q11" s="4" t="n">
+        <v>0.5</v>
+      </c>
       <c r="R11" s="4" t="s">
         <v>55</v>
       </c>
@@ -4945,7 +4949,7 @@
       <c r="A71" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:Q67"/>
+  <autoFilter ref="B1:P67"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>